<commit_message>
Make GMH parameters consistent
For GMH 627,628, changed 'correction' to 'T_correction' to match with
GMH367.
</commit_message>
<xml_diff>
--- a/HRBC_template.xlsx
+++ b/HRBC_template.xlsx
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="361">
   <si>
     <t>start_row</t>
   </si>
@@ -950,9 +950,6 @@
   </si>
   <si>
     <t>SR104t_Tref_LV</t>
-  </si>
-  <si>
-    <t>correction</t>
   </si>
   <si>
     <t>GMH627_cor</t>
@@ -1679,6 +1676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1686,7 +1684,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2098,21 +2095,21 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="M3" s="54" t="s">
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="M3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="54" t="s">
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
       <c r="S3" t="s">
         <v>11</v>
       </c>
@@ -2125,11 +2122,11 @@
       <c r="V3" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="54" t="s">
+      <c r="W3" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
       <c r="Z3" t="s">
         <v>16</v>
       </c>
@@ -5939,7 +5936,7 @@
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="540" activePane="bottomLeft"/>
       <selection activeCell="F2" sqref="F2"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49:F49"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6276,7 +6273,7 @@
         <v>169</v>
       </c>
       <c r="J10" t="s">
-        <v>244</v>
+        <v>211</v>
       </c>
       <c r="K10" s="21">
         <v>-1E-3</v>
@@ -6288,13 +6285,13 @@
         <v>208</v>
       </c>
       <c r="N10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O10" t="s">
         <v>213</v>
       </c>
       <c r="R10" s="37" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -6314,7 +6311,7 @@
         <v>208</v>
       </c>
       <c r="F11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I11" t="s">
         <v>169</v>
@@ -6329,10 +6326,10 @@
         <v>228</v>
       </c>
       <c r="R11" t="s">
+        <v>247</v>
+      </c>
+      <c r="S11" s="37" t="s">
         <v>248</v>
-      </c>
-      <c r="S11" s="37" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -6352,7 +6349,7 @@
         <v>208</v>
       </c>
       <c r="F12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I12" t="s">
         <v>169</v>
@@ -6361,16 +6358,16 @@
         <v>231</v>
       </c>
       <c r="K12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O12" t="s">
         <v>228</v>
       </c>
       <c r="S12" t="s">
+        <v>251</v>
+      </c>
+      <c r="T12" s="37" t="s">
         <v>252</v>
-      </c>
-      <c r="T12" s="37" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -6390,13 +6387,13 @@
         <v>235</v>
       </c>
       <c r="K13" t="s">
+        <v>253</v>
+      </c>
+      <c r="T13" t="s">
         <v>254</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" s="37" t="s">
         <v>255</v>
-      </c>
-      <c r="U13" s="37" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -6426,10 +6423,10 @@
       <c r="M14" s="36"/>
       <c r="N14" s="36"/>
       <c r="O14" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="T14" s="37" t="s">
         <v>257</v>
-      </c>
-      <c r="T14" s="37" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -6449,13 +6446,13 @@
         <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I15" t="s">
         <v>170</v>
       </c>
       <c r="J15" t="s">
-        <v>244</v>
+        <v>211</v>
       </c>
       <c r="K15" s="21">
         <v>-5.0000000000000001E-4</v>
@@ -6467,13 +6464,13 @@
         <v>208</v>
       </c>
       <c r="N15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O15" t="s">
         <v>213</v>
       </c>
       <c r="S15" s="37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="T15" s="37"/>
     </row>
@@ -6494,7 +6491,7 @@
         <v>208</v>
       </c>
       <c r="F16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I16" t="s">
         <v>170</v>
@@ -6509,7 +6506,7 @@
         <v>228</v>
       </c>
       <c r="S16" s="37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="T16" s="37"/>
     </row>
@@ -6518,7 +6515,7 @@
         <v>186</v>
       </c>
       <c r="B17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C17" s="21">
         <v>5</v>
@@ -6530,7 +6527,7 @@
         <v>208</v>
       </c>
       <c r="F17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I17" t="s">
         <v>170</v>
@@ -6539,13 +6536,13 @@
         <v>231</v>
       </c>
       <c r="K17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O17" t="s">
         <v>228</v>
       </c>
       <c r="S17" s="37" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="T17" s="37"/>
     </row>
@@ -6554,7 +6551,7 @@
         <v>186</v>
       </c>
       <c r="B18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C18">
         <v>9999.9992600000005</v>
@@ -6566,7 +6563,7 @@
         <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I18" t="s">
         <v>170</v>
@@ -6575,13 +6572,13 @@
         <v>235</v>
       </c>
       <c r="K18" t="s">
+        <v>269</v>
+      </c>
+      <c r="S18" t="s">
+        <v>251</v>
+      </c>
+      <c r="T18" t="s">
         <v>270</v>
-      </c>
-      <c r="S18" t="s">
-        <v>252</v>
-      </c>
-      <c r="T18" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -6589,7 +6586,7 @@
         <v>186</v>
       </c>
       <c r="B19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C19" s="10">
         <v>20</v>
@@ -6601,7 +6598,7 @@
         <v>208</v>
       </c>
       <c r="F19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I19" s="36" t="s">
         <v>170</v>
@@ -6616,10 +6613,10 @@
       <c r="M19" s="36"/>
       <c r="N19" s="36"/>
       <c r="O19" s="36" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="T19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -6627,7 +6624,7 @@
         <v>186</v>
       </c>
       <c r="B20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -6639,7 +6636,7 @@
         <v>208</v>
       </c>
       <c r="F20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I20" t="s">
         <v>10</v>
@@ -6651,7 +6648,7 @@
         <v>2</v>
       </c>
       <c r="S20" s="37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -6671,7 +6668,7 @@
         <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I21" t="s">
         <v>10</v>
@@ -6680,13 +6677,13 @@
         <v>231</v>
       </c>
       <c r="K21" t="s">
+        <v>278</v>
+      </c>
+      <c r="S21" t="s">
+        <v>251</v>
+      </c>
+      <c r="T21" t="s">
         <v>279</v>
-      </c>
-      <c r="S21" t="s">
-        <v>252</v>
-      </c>
-      <c r="T21" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -6706,7 +6703,7 @@
         <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I22" t="s">
         <v>10</v>
@@ -6718,7 +6715,7 @@
         <v>66</v>
       </c>
       <c r="T22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -6726,7 +6723,7 @@
         <v>186</v>
       </c>
       <c r="B23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -6738,7 +6735,7 @@
         <v>208</v>
       </c>
       <c r="F23" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I23" s="36" t="s">
         <v>10</v>
@@ -6747,17 +6744,17 @@
         <v>240</v>
       </c>
       <c r="K23" s="36" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L23" s="36"/>
       <c r="M23" s="36"/>
       <c r="N23" s="36"/>
       <c r="O23" s="36"/>
       <c r="T23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="U23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -6801,7 +6798,7 @@
         <v>231</v>
       </c>
       <c r="K25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -6823,12 +6820,12 @@
         <v>240</v>
       </c>
       <c r="K27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I28" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J28" s="13" t="s">
         <v>227</v>
@@ -6843,18 +6840,18 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I29" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J29" t="s">
         <v>231</v>
       </c>
       <c r="K29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J30" t="s">
         <v>235</v>
@@ -6865,13 +6862,13 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I31" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J31" s="36" t="s">
         <v>240</v>
       </c>
       <c r="K31" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L31" s="36"/>
       <c r="M31" s="36"/>
@@ -6897,7 +6894,7 @@
         <v>231</v>
       </c>
       <c r="K33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="34" spans="9:15" x14ac:dyDescent="0.25">
@@ -6919,7 +6916,7 @@
         <v>240</v>
       </c>
       <c r="K35" s="36" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L35" s="36"/>
       <c r="M35" s="36"/>
@@ -6931,7 +6928,7 @@
         <v>37</v>
       </c>
       <c r="J36" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -6948,7 +6945,7 @@
         <v>37</v>
       </c>
       <c r="J37" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -6965,7 +6962,7 @@
         <v>37</v>
       </c>
       <c r="J38" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -6982,7 +6979,7 @@
         <v>37</v>
       </c>
       <c r="J39" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -6999,7 +6996,7 @@
         <v>37</v>
       </c>
       <c r="J40" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -7016,7 +7013,7 @@
         <v>37</v>
       </c>
       <c r="J41" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K41">
         <v>0</v>
@@ -7033,7 +7030,7 @@
         <v>37</v>
       </c>
       <c r="J42" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -7050,7 +7047,7 @@
         <v>37</v>
       </c>
       <c r="J43" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -7081,7 +7078,7 @@
         <v>231</v>
       </c>
       <c r="K45" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="46" spans="9:15" x14ac:dyDescent="0.25">
@@ -7092,7 +7089,7 @@
         <v>235</v>
       </c>
       <c r="K46" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="47" spans="9:15" x14ac:dyDescent="0.25">
@@ -7110,10 +7107,10 @@
     </row>
     <row r="48" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K48">
         <v>0</v>
@@ -7127,10 +7124,10 @@
     </row>
     <row r="49" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I49" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J49" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K49">
         <v>0</v>
@@ -7144,10 +7141,10 @@
     </row>
     <row r="50" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I50" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J50" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K50">
         <v>0</v>
@@ -7161,7 +7158,7 @@
     </row>
     <row r="51" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I51" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J51" t="s">
         <v>227</v>
@@ -7173,52 +7170,52 @@
     </row>
     <row r="52" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I52" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J52" t="s">
         <v>231</v>
       </c>
       <c r="K52" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M52" s="40"/>
     </row>
     <row r="53" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I53" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J53" t="s">
+        <v>301</v>
+      </c>
+      <c r="K53" t="s">
         <v>302</v>
-      </c>
-      <c r="K53" t="s">
-        <v>303</v>
       </c>
       <c r="M53" s="40"/>
     </row>
     <row r="54" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J54" t="s">
         <v>235</v>
       </c>
       <c r="K54" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M54" s="40"/>
     </row>
     <row r="55" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I55" s="36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J55" s="36" t="s">
         <v>240</v>
       </c>
       <c r="K55" s="36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L55" s="36"/>
-      <c r="M55" s="55"/>
+      <c r="M55" s="52"/>
       <c r="N55" s="36"/>
       <c r="O55" s="36"/>
     </row>
@@ -7227,7 +7224,7 @@
         <v>57</v>
       </c>
       <c r="J56" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K56">
         <v>0</v>
@@ -7244,7 +7241,7 @@
         <v>57</v>
       </c>
       <c r="J57" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -7261,7 +7258,7 @@
         <v>57</v>
       </c>
       <c r="J58" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K58">
         <v>0</v>
@@ -7292,7 +7289,7 @@
         <v>231</v>
       </c>
       <c r="K60" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="61" spans="9:15" x14ac:dyDescent="0.25">
@@ -7300,10 +7297,10 @@
         <v>57</v>
       </c>
       <c r="J61" t="s">
+        <v>301</v>
+      </c>
+      <c r="K61" t="s">
         <v>302</v>
-      </c>
-      <c r="K61" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="62" spans="9:15" x14ac:dyDescent="0.25">
@@ -7314,7 +7311,7 @@
         <v>235</v>
       </c>
       <c r="K62" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="63" spans="9:15" x14ac:dyDescent="0.25">
@@ -7325,15 +7322,15 @@
         <v>240</v>
       </c>
       <c r="K63" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="64" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I64" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J64" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K64" s="38">
         <v>0</v>
@@ -7349,10 +7346,10 @@
     </row>
     <row r="65" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I65" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J65" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K65" s="39">
         <v>-5.6799999999999998E-5</v>
@@ -7364,15 +7361,15 @@
         <v>208</v>
       </c>
       <c r="N65" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="I66" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J66" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K66" s="39">
         <v>-5.63E-5</v>
@@ -7384,15 +7381,15 @@
         <v>208</v>
       </c>
       <c r="N66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="67" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I67" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J67" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K67" s="40">
         <v>0</v>
@@ -7404,15 +7401,15 @@
         <v>7</v>
       </c>
       <c r="N67" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="68" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I68" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J68" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K68" s="39">
         <v>2.2210000000000001E-7</v>
@@ -7424,18 +7421,18 @@
         <v>7</v>
       </c>
       <c r="N68" t="s">
+        <v>311</v>
+      </c>
+      <c r="O68" t="s">
         <v>312</v>
-      </c>
-      <c r="O68" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="69" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I69" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J69" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K69" s="39">
         <v>4.8090000000000002E-7</v>
@@ -7447,18 +7444,18 @@
         <v>208</v>
       </c>
       <c r="N69" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O69" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="70" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I70" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J70" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K70" s="40">
         <v>0</v>
@@ -7470,18 +7467,18 @@
         <v>8</v>
       </c>
       <c r="N70" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O70" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="71" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I71" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J71" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K71" s="40">
         <v>0</v>
@@ -7493,15 +7490,15 @@
         <v>8</v>
       </c>
       <c r="N71" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O71" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="72" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I72" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J72" t="s">
         <v>227</v>
@@ -7512,46 +7509,46 @@
     </row>
     <row r="73" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I73" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J73" t="s">
         <v>231</v>
       </c>
       <c r="K73" s="40" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="74" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I74" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J74" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K74" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="75" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I75" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J75" t="s">
         <v>235</v>
       </c>
       <c r="K75" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="76" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I76" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J76" s="36" t="s">
         <v>240</v>
       </c>
       <c r="K76" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L76" s="36"/>
       <c r="M76" s="36"/>
@@ -7560,10 +7557,10 @@
     </row>
     <row r="77" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I77" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J77" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K77" s="40">
         <v>0</v>
@@ -7577,10 +7574,10 @@
     </row>
     <row r="78" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I78" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J78" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K78" s="39">
         <v>-5.6799999999999998E-5</v>
@@ -7592,15 +7589,15 @@
         <v>208</v>
       </c>
       <c r="N78" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="79" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I79" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J79" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K79" s="39">
         <v>-5.63E-5</v>
@@ -7612,15 +7609,15 @@
         <v>208</v>
       </c>
       <c r="N79" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="80" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I80" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J80" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K80" s="40">
         <v>0</v>
@@ -7632,18 +7629,18 @@
         <v>7</v>
       </c>
       <c r="N80" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="O80" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="81" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I81" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J81" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K81" s="39">
         <v>2.2210000000000001E-7</v>
@@ -7655,18 +7652,18 @@
         <v>7</v>
       </c>
       <c r="N81" t="s">
+        <v>311</v>
+      </c>
+      <c r="O81" t="s">
         <v>312</v>
-      </c>
-      <c r="O81" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="82" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I82" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J82" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K82" s="39">
         <v>4.8090000000000002E-7</v>
@@ -7678,18 +7675,18 @@
         <v>208</v>
       </c>
       <c r="N82" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O82" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="83" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I83" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J83" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K83" s="40">
         <v>0</v>
@@ -7701,18 +7698,18 @@
         <v>8</v>
       </c>
       <c r="N83" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O83" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="84" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I84" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J84" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K84" s="40">
         <v>0</v>
@@ -7724,12 +7721,12 @@
         <v>8</v>
       </c>
       <c r="N84" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="85" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I85" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J85" t="s">
         <v>227</v>
@@ -7740,46 +7737,46 @@
     </row>
     <row r="86" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I86" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J86" t="s">
         <v>231</v>
       </c>
       <c r="K86" s="40" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="87" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I87" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J87" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K87" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="88" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I88" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J88" t="s">
         <v>235</v>
       </c>
       <c r="K88" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="89" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I89" s="36" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J89" s="36" t="s">
         <v>240</v>
       </c>
       <c r="K89" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L89" s="14"/>
       <c r="M89" s="14"/>
@@ -7791,7 +7788,7 @@
         <v>171</v>
       </c>
       <c r="J90" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K90" s="40">
         <v>0</v>
@@ -7808,7 +7805,7 @@
         <v>171</v>
       </c>
       <c r="J91" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K91" s="39">
         <v>-5.6799999999999998E-5</v>
@@ -7820,7 +7817,7 @@
         <v>208</v>
       </c>
       <c r="N91" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="92" spans="9:15" x14ac:dyDescent="0.25">
@@ -7828,7 +7825,7 @@
         <v>171</v>
       </c>
       <c r="J92" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K92" s="39">
         <v>-5.63E-5</v>
@@ -7840,7 +7837,7 @@
         <v>208</v>
       </c>
       <c r="N92" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="93" spans="9:15" x14ac:dyDescent="0.25">
@@ -7848,7 +7845,7 @@
         <v>171</v>
       </c>
       <c r="J93" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K93" s="40">
         <v>0</v>
@@ -7860,10 +7857,10 @@
         <v>7</v>
       </c>
       <c r="N93" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="O93" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="94" spans="9:15" x14ac:dyDescent="0.25">
@@ -7871,7 +7868,7 @@
         <v>171</v>
       </c>
       <c r="J94" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K94" s="39">
         <v>2.2210000000000001E-7</v>
@@ -7883,10 +7880,10 @@
         <v>7</v>
       </c>
       <c r="N94" t="s">
+        <v>311</v>
+      </c>
+      <c r="O94" t="s">
         <v>312</v>
-      </c>
-      <c r="O94" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="95" spans="9:15" x14ac:dyDescent="0.25">
@@ -7894,7 +7891,7 @@
         <v>171</v>
       </c>
       <c r="J95" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K95" s="39">
         <v>4.8090000000000002E-7</v>
@@ -7906,10 +7903,10 @@
         <v>208</v>
       </c>
       <c r="N95" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O95" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="96" spans="9:15" x14ac:dyDescent="0.25">
@@ -7917,7 +7914,7 @@
         <v>171</v>
       </c>
       <c r="J96" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K96" s="40">
         <v>0</v>
@@ -7929,10 +7926,10 @@
         <v>8</v>
       </c>
       <c r="N96" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O96" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="97" spans="9:15" x14ac:dyDescent="0.25">
@@ -7940,7 +7937,7 @@
         <v>171</v>
       </c>
       <c r="J97" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K97" s="40">
         <v>0</v>
@@ -7952,7 +7949,7 @@
         <v>8</v>
       </c>
       <c r="N97" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="98" spans="9:15" x14ac:dyDescent="0.25">
@@ -7974,7 +7971,7 @@
         <v>231</v>
       </c>
       <c r="K99" s="40" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="100" spans="9:15" x14ac:dyDescent="0.25">
@@ -7982,10 +7979,10 @@
         <v>171</v>
       </c>
       <c r="J100" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K100" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="101" spans="9:15" x14ac:dyDescent="0.25">
@@ -7996,7 +7993,7 @@
         <v>235</v>
       </c>
       <c r="K101" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="102" spans="9:15" x14ac:dyDescent="0.25">
@@ -8007,7 +8004,7 @@
         <v>240</v>
       </c>
       <c r="K102" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L102" s="36"/>
       <c r="M102" s="36"/>
@@ -8019,7 +8016,7 @@
         <v>62</v>
       </c>
       <c r="J103" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K103" s="40">
         <v>0</v>
@@ -8036,7 +8033,7 @@
         <v>62</v>
       </c>
       <c r="J104" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K104" s="39">
         <v>-5.6799999999999998E-5</v>
@@ -8048,7 +8045,7 @@
         <v>208</v>
       </c>
       <c r="N104" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="105" spans="9:15" x14ac:dyDescent="0.25">
@@ -8056,7 +8053,7 @@
         <v>62</v>
       </c>
       <c r="J105" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K105" s="39">
         <v>-5.63E-5</v>
@@ -8068,7 +8065,7 @@
         <v>208</v>
       </c>
       <c r="N105" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="106" spans="9:15" x14ac:dyDescent="0.25">
@@ -8076,7 +8073,7 @@
         <v>62</v>
       </c>
       <c r="J106" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K106" s="40">
         <v>0</v>
@@ -8088,10 +8085,10 @@
         <v>7</v>
       </c>
       <c r="N106" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="O106" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="107" spans="9:15" x14ac:dyDescent="0.25">
@@ -8099,7 +8096,7 @@
         <v>62</v>
       </c>
       <c r="J107" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K107" s="39">
         <v>2.2210000000000001E-7</v>
@@ -8111,10 +8108,10 @@
         <v>7</v>
       </c>
       <c r="N107" t="s">
+        <v>311</v>
+      </c>
+      <c r="O107" t="s">
         <v>312</v>
-      </c>
-      <c r="O107" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="108" spans="9:15" x14ac:dyDescent="0.25">
@@ -8122,7 +8119,7 @@
         <v>62</v>
       </c>
       <c r="J108" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K108" s="39">
         <v>4.8090000000000002E-7</v>
@@ -8134,10 +8131,10 @@
         <v>208</v>
       </c>
       <c r="N108" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O108" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="109" spans="9:15" x14ac:dyDescent="0.25">
@@ -8145,7 +8142,7 @@
         <v>62</v>
       </c>
       <c r="J109" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K109" s="40">
         <v>0</v>
@@ -8157,10 +8154,10 @@
         <v>8</v>
       </c>
       <c r="N109" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O109" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="110" spans="9:15" x14ac:dyDescent="0.25">
@@ -8168,7 +8165,7 @@
         <v>62</v>
       </c>
       <c r="J110" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K110" s="40">
         <v>0</v>
@@ -8180,7 +8177,7 @@
         <v>8</v>
       </c>
       <c r="N110" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="111" spans="9:15" x14ac:dyDescent="0.25">
@@ -8202,7 +8199,7 @@
         <v>231</v>
       </c>
       <c r="K112" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="113" spans="9:15" x14ac:dyDescent="0.25">
@@ -8210,10 +8207,10 @@
         <v>62</v>
       </c>
       <c r="J113" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K113" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="114" spans="9:15" x14ac:dyDescent="0.25">
@@ -8224,7 +8221,7 @@
         <v>235</v>
       </c>
       <c r="K114" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="115" spans="9:15" x14ac:dyDescent="0.25">
@@ -8235,7 +8232,7 @@
         <v>240</v>
       </c>
       <c r="K115" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L115" s="36"/>
       <c r="M115" s="36"/>
@@ -8247,7 +8244,7 @@
         <v>71</v>
       </c>
       <c r="J116" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K116" s="40">
         <v>0</v>
@@ -8264,7 +8261,7 @@
         <v>71</v>
       </c>
       <c r="J117" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K117" s="39">
         <v>-5.6799999999999998E-5</v>
@@ -8276,7 +8273,7 @@
         <v>208</v>
       </c>
       <c r="N117" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="118" spans="9:15" x14ac:dyDescent="0.25">
@@ -8284,7 +8281,7 @@
         <v>71</v>
       </c>
       <c r="J118" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K118" s="39">
         <v>-5.63E-5</v>
@@ -8296,7 +8293,7 @@
         <v>208</v>
       </c>
       <c r="N118" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="119" spans="9:15" x14ac:dyDescent="0.25">
@@ -8304,7 +8301,7 @@
         <v>71</v>
       </c>
       <c r="J119" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K119" s="40">
         <v>0</v>
@@ -8316,10 +8313,10 @@
         <v>7</v>
       </c>
       <c r="N119" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="O119" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="120" spans="9:15" x14ac:dyDescent="0.25">
@@ -8327,7 +8324,7 @@
         <v>71</v>
       </c>
       <c r="J120" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K120" s="39">
         <v>2.2210000000000001E-7</v>
@@ -8339,10 +8336,10 @@
         <v>7</v>
       </c>
       <c r="N120" t="s">
+        <v>311</v>
+      </c>
+      <c r="O120" t="s">
         <v>312</v>
-      </c>
-      <c r="O120" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="121" spans="9:15" x14ac:dyDescent="0.25">
@@ -8350,7 +8347,7 @@
         <v>71</v>
       </c>
       <c r="J121" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K121" s="39">
         <v>4.8090000000000002E-7</v>
@@ -8362,10 +8359,10 @@
         <v>208</v>
       </c>
       <c r="N121" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O121" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="122" spans="9:15" x14ac:dyDescent="0.25">
@@ -8373,7 +8370,7 @@
         <v>71</v>
       </c>
       <c r="J122" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K122" s="40">
         <v>0</v>
@@ -8385,10 +8382,10 @@
         <v>8</v>
       </c>
       <c r="N122" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O122" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="123" spans="9:15" x14ac:dyDescent="0.25">
@@ -8396,7 +8393,7 @@
         <v>71</v>
       </c>
       <c r="J123" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K123" s="40">
         <v>0</v>
@@ -8408,7 +8405,7 @@
         <v>8</v>
       </c>
       <c r="N123" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="124" spans="9:15" x14ac:dyDescent="0.25">
@@ -8430,7 +8427,7 @@
         <v>231</v>
       </c>
       <c r="K125" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="126" spans="9:15" x14ac:dyDescent="0.25">
@@ -8438,10 +8435,10 @@
         <v>71</v>
       </c>
       <c r="J126" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K126" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="127" spans="9:15" x14ac:dyDescent="0.25">
@@ -8452,7 +8449,7 @@
         <v>235</v>
       </c>
       <c r="K127" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="128" spans="9:15" x14ac:dyDescent="0.25">
@@ -8463,7 +8460,7 @@
         <v>240</v>
       </c>
       <c r="K128" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L128" s="36"/>
       <c r="M128" s="36"/>
@@ -8491,7 +8488,7 @@
         <v>231</v>
       </c>
       <c r="K130" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L130" s="39"/>
       <c r="M130" s="40"/>
@@ -8501,16 +8498,16 @@
         <v>42</v>
       </c>
       <c r="J131" t="s">
+        <v>337</v>
+      </c>
+      <c r="K131" t="s">
         <v>338</v>
       </c>
-      <c r="K131" t="s">
+      <c r="L131" s="19" t="s">
         <v>339</v>
       </c>
-      <c r="L131" s="19" t="s">
+      <c r="M131" s="20" t="s">
         <v>340</v>
-      </c>
-      <c r="M131" s="20" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="132" spans="9:15" x14ac:dyDescent="0.25">
@@ -8518,13 +8515,13 @@
         <v>42</v>
       </c>
       <c r="J132" t="s">
+        <v>341</v>
+      </c>
+      <c r="K132" t="s">
         <v>342</v>
       </c>
-      <c r="K132" t="s">
+      <c r="L132" s="19" t="s">
         <v>343</v>
-      </c>
-      <c r="L132" s="19" t="s">
-        <v>344</v>
       </c>
       <c r="M132" s="40"/>
     </row>
@@ -8533,10 +8530,10 @@
         <v>42</v>
       </c>
       <c r="J133" t="s">
+        <v>344</v>
+      </c>
+      <c r="K133" t="s">
         <v>345</v>
-      </c>
-      <c r="K133" t="s">
-        <v>346</v>
       </c>
       <c r="L133" s="39"/>
       <c r="M133" s="40"/>
@@ -8546,10 +8543,10 @@
         <v>42</v>
       </c>
       <c r="J134" t="s">
+        <v>346</v>
+      </c>
+      <c r="K134" t="s">
         <v>347</v>
-      </c>
-      <c r="K134" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="135" spans="9:15" x14ac:dyDescent="0.25">
@@ -8560,7 +8557,7 @@
         <v>235</v>
       </c>
       <c r="K135" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="136" spans="9:15" x14ac:dyDescent="0.25">
@@ -8571,7 +8568,7 @@
         <v>240</v>
       </c>
       <c r="K136" s="36" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L136" s="36"/>
       <c r="M136" s="36"/>
@@ -8598,7 +8595,7 @@
         <v>231</v>
       </c>
       <c r="K138" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L138" s="39"/>
     </row>
@@ -8607,10 +8604,10 @@
         <v>32</v>
       </c>
       <c r="J139" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K139" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L139" s="39"/>
     </row>
@@ -8619,13 +8616,13 @@
         <v>32</v>
       </c>
       <c r="J140" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K140" t="s">
+        <v>352</v>
+      </c>
+      <c r="L140" s="19" t="s">
         <v>353</v>
-      </c>
-      <c r="L140" s="19" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="141" spans="9:15" x14ac:dyDescent="0.25">
@@ -8633,10 +8630,10 @@
         <v>32</v>
       </c>
       <c r="J141" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K141" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L141" s="39"/>
     </row>
@@ -8645,10 +8642,10 @@
         <v>32</v>
       </c>
       <c r="J142" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K142" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="143" spans="9:15" x14ac:dyDescent="0.25">
@@ -8656,13 +8653,13 @@
         <v>32</v>
       </c>
       <c r="J143" t="s">
+        <v>356</v>
+      </c>
+      <c r="K143" t="s">
         <v>357</v>
       </c>
-      <c r="K143" t="s">
+      <c r="L143" t="s">
         <v>358</v>
-      </c>
-      <c r="L143" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="144" spans="9:15" x14ac:dyDescent="0.25">
@@ -8673,7 +8670,7 @@
         <v>235</v>
       </c>
       <c r="K144" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="145" spans="9:15" x14ac:dyDescent="0.25">
@@ -8684,7 +8681,7 @@
         <v>240</v>
       </c>
       <c r="K145" s="36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L145" s="36"/>
       <c r="M145" s="36"/>

</xml_diff>

<commit_message>
Remove refs to device.is_open parameter
Also, Rlink run changed Excel sheet.
</commit_message>
<xml_diff>
--- a/HRBC_template.xlsx
+++ b/HRBC_template.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="361">
   <si>
     <t>start_row</t>
   </si>
@@ -624,34 +624,31 @@
     <t>R1: TestR1 1G monitored by GMH: s/n627. R2: TestR2 100M monitored by GMH: s/n628</t>
   </si>
   <si>
-    <t>18/05/2017 16:58:09</t>
-  </si>
-  <si>
-    <t>18/05/2017 16:58:14</t>
-  </si>
-  <si>
-    <t>18/05/2017 16:58:04</t>
-  </si>
-  <si>
-    <t>R1: CHANGE_THIS! 1G monitored by GMH: s/n627. R2: CHANGE_THIS! 1M monitored by GMH: s/n628</t>
-  </si>
-  <si>
-    <t>18/05/2017 16:58:40</t>
-  </si>
-  <si>
-    <t>18/05/2017 16:58:46</t>
-  </si>
-  <si>
-    <t>18/05/2017 16:58:36</t>
-  </si>
-  <si>
-    <t>18/05/2017 16:59:11</t>
-  </si>
-  <si>
-    <t>18/05/2017 16:59:16</t>
-  </si>
-  <si>
-    <t>18/05/2017 16:59:06</t>
+    <t>25/05/2017 14:38:05</t>
+  </si>
+  <si>
+    <t>25/05/2017 14:38:11</t>
+  </si>
+  <si>
+    <t>25/05/2017 14:38:01</t>
+  </si>
+  <si>
+    <t>25/05/2017 14:38:39</t>
+  </si>
+  <si>
+    <t>25/05/2017 14:38:45</t>
+  </si>
+  <si>
+    <t>25/05/2017 14:38:35</t>
+  </si>
+  <si>
+    <t>25/05/2017 14:39:12</t>
+  </si>
+  <si>
+    <t>25/05/2017 14:39:17</t>
+  </si>
+  <si>
+    <t>25/05/2017 14:39:07</t>
   </si>
   <si>
     <t>GMH: s/n627</t>
@@ -723,16 +720,13 @@
     <t>Rd</t>
   </si>
   <si>
-    <t>HRBC.v0.4 CHANGE_THIS! 1G:CHANGE_THIS! 1M 18/05/2017 16:57:02</t>
-  </si>
-  <si>
-    <t>18/05/2017 17:01:29</t>
-  </si>
-  <si>
-    <t>CHANGE_THIS! 1G</t>
-  </si>
-  <si>
-    <t>CHANGE_THIS! 1M</t>
+    <t>25/05/2017 14:40:22</t>
+  </si>
+  <si>
+    <t>TestR1 1G</t>
+  </si>
+  <si>
+    <t>TestR2 100M</t>
   </si>
   <si>
     <t>Resistor Info:</t>
@@ -1231,33 +1225,6 @@
   </si>
   <si>
     <t>UNUSED F5520A</t>
-  </si>
-  <si>
-    <t>25/05/2017 14:38:05</t>
-  </si>
-  <si>
-    <t>25/05/2017 14:38:11</t>
-  </si>
-  <si>
-    <t>25/05/2017 14:38:01</t>
-  </si>
-  <si>
-    <t>25/05/2017 14:38:39</t>
-  </si>
-  <si>
-    <t>25/05/2017 14:38:45</t>
-  </si>
-  <si>
-    <t>25/05/2017 14:38:35</t>
-  </si>
-  <si>
-    <t>25/05/2017 14:39:12</t>
-  </si>
-  <si>
-    <t>25/05/2017 14:39:17</t>
-  </si>
-  <si>
-    <t>25/05/2017 14:39:07</t>
   </si>
 </sst>
 </file>
@@ -1271,7 +1238,7 @@
     <numFmt formatCode="0.00000" numFmtId="167"/>
     <numFmt formatCode="0.0000" numFmtId="168"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1401,6 +1368,18 @@
       <family val="2"/>
       <b val="1"/>
       <color rgb="00000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="00FF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="000000FF"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -1623,7 +1602,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0"/>
@@ -1698,6 +1677,8 @@
     <xf borderId="19" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="20" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="21" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -4695,7 +4676,7 @@
         <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>363</v>
+        <v>160</v>
       </c>
       <c r="H45" t="n">
         <v>1.000375572074</v>
@@ -4704,7 +4685,7 @@
         <v>1.142601011611787e-05</v>
       </c>
       <c r="M45" t="s">
-        <v>364</v>
+        <v>161</v>
       </c>
       <c r="N45" t="n">
         <v>-5.779654168612317e-07</v>
@@ -4713,7 +4694,7 @@
         <v>1.18572366257827e-06</v>
       </c>
       <c r="P45" t="s">
-        <v>365</v>
+        <v>162</v>
       </c>
       <c r="Q45" t="n">
         <v>-9.999991826104967</v>
@@ -4772,7 +4753,7 @@
         <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>366</v>
+        <v>163</v>
       </c>
       <c r="H46" t="n">
         <v>-1.000368184232376</v>
@@ -4781,7 +4762,7 @@
         <v>7.838164654959872e-06</v>
       </c>
       <c r="M46" t="s">
-        <v>367</v>
+        <v>164</v>
       </c>
       <c r="N46" t="n">
         <v>2.728296693586928e-08</v>
@@ -4790,7 +4771,7 @@
         <v>8.9845151580551e-07</v>
       </c>
       <c r="P46" t="s">
-        <v>368</v>
+        <v>165</v>
       </c>
       <c r="Q46" t="n">
         <v>10.00002011031934</v>
@@ -4849,7 +4830,7 @@
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>369</v>
+        <v>166</v>
       </c>
       <c r="H47" t="n">
         <v>-1.010370466552908</v>
@@ -4858,7 +4839,7 @@
         <v>1.081586397589585e-05</v>
       </c>
       <c r="M47" t="s">
-        <v>370</v>
+        <v>167</v>
       </c>
       <c r="N47" t="n">
         <v>-2.728360361729995e-07</v>
@@ -4867,7 +4848,7 @@
         <v>6.574043515367278e-07</v>
       </c>
       <c r="P47" t="s">
-        <v>371</v>
+        <v>168</v>
       </c>
       <c r="Q47" t="n">
         <v>9.999961668555143</v>
@@ -4903,7 +4884,7 @@
         <v>46</v>
       </c>
       <c s="61" r="AD47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row s="55" r="48" spans="1:35">
@@ -4911,7 +4892,7 @@
         <v>51</v>
       </c>
       <c s="61" r="AD48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row s="55" r="49" spans="1:35">
@@ -4927,15 +4908,15 @@
         <v>61</v>
       </c>
       <c s="61" r="AD50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row s="55" r="51" spans="1:35">
       <c s="60" r="AC51" t="s">
+        <v>172</v>
+      </c>
+      <c s="61" r="AD51" t="s">
         <v>173</v>
-      </c>
-      <c s="61" r="AD51" t="s">
-        <v>174</v>
       </c>
     </row>
     <row s="55" r="52" spans="1:35">
@@ -4993,27 +4974,27 @@
     <col bestFit="1" customWidth="1" max="8" min="8" style="55" width="14.7109375"/>
     <col bestFit="1" customWidth="1" max="9" min="9" style="55" width="15.42578125"/>
     <col bestFit="1" customWidth="1" max="10" min="10" style="55" width="14.7109375"/>
-    <col customWidth="1" hidden="1" max="11" min="11" style="55"/>
+    <col hidden="1" max="11" min="11" style="55"/>
     <col bestFit="1" customWidth="1" max="12" min="12" style="55" width="15.42578125"/>
     <col bestFit="1" customWidth="1" max="13" min="13" style="55" width="14.7109375"/>
     <col bestFit="1" customWidth="1" max="14" min="14" style="55" width="15.42578125"/>
-    <col customWidth="1" hidden="1" max="20" min="15" style="55"/>
-    <col customWidth="1" hidden="1" max="20" min="15" style="55"/>
-    <col customWidth="1" hidden="1" max="20" min="15" style="55"/>
-    <col customWidth="1" hidden="1" max="20" min="15" style="55"/>
-    <col customWidth="1" hidden="1" max="20" min="15" style="55"/>
-    <col customWidth="1" hidden="1" max="20" min="15" style="55"/>
+    <col hidden="1" max="20" min="15" style="55"/>
+    <col hidden="1" max="20" min="15" style="55"/>
+    <col hidden="1" max="20" min="15" style="55"/>
+    <col hidden="1" max="20" min="15" style="55"/>
+    <col hidden="1" max="20" min="15" style="55"/>
+    <col hidden="1" max="20" min="15" style="55"/>
   </cols>
   <sheetData>
     <row s="55" r="1" spans="1:20">
       <c s="5" r="A1" t="s">
+        <v>174</v>
+      </c>
+      <c s="3" r="B1" t="n">
+        <v>45</v>
+      </c>
+      <c s="6" r="C1" t="s">
         <v>175</v>
-      </c>
-      <c s="3" r="B1" t="n">
-        <v>28</v>
-      </c>
-      <c s="6" r="C1" t="s">
-        <v>176</v>
       </c>
       <c s="4" r="D1" t="n">
         <v>10</v>
@@ -5021,13 +5002,13 @@
     </row>
     <row s="55" r="2" spans="1:20">
       <c s="5" r="A2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c s="3" r="B2" t="n">
         <v>10</v>
       </c>
       <c s="6" r="C2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c s="4" r="D2" t="n">
         <v>1</v>
@@ -5035,7 +5016,7 @@
     </row>
     <row s="55" r="3" spans="1:20">
       <c s="5" r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c s="3" r="B3" t="n">
         <v>10</v>
@@ -5061,18 +5042,18 @@
         <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row s="55" r="7" spans="1:20">
       <c r="A7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" t="s">
         <v>181</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>182</v>
-      </c>
-      <c r="D7" t="s">
-        <v>183</v>
       </c>
       <c r="M7" t="n">
         <v>0.0001</v>
@@ -5080,10 +5061,10 @@
     </row>
     <row s="55" r="8" spans="1:20">
       <c r="A8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" t="s">
         <v>184</v>
-      </c>
-      <c r="B8" t="s">
-        <v>185</v>
       </c>
       <c r="C8" t="n">
         <v>100000</v>
@@ -5094,10 +5075,10 @@
     </row>
     <row s="55" r="9" spans="1:20">
       <c r="A9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" t="s">
         <v>186</v>
-      </c>
-      <c r="B9" t="s">
-        <v>187</v>
       </c>
       <c r="C9" t="n">
         <v>10000</v>
@@ -5108,40 +5089,40 @@
     </row>
     <row s="55" r="10" spans="1:20">
       <c s="34" r="A10" t="s">
+        <v>187</v>
+      </c>
+      <c s="35" r="B10" t="s">
         <v>188</v>
       </c>
-      <c s="35" r="B10" t="s">
+      <c s="34" r="C10" t="s">
+        <v>187</v>
+      </c>
+      <c s="35" r="D10" t="s">
+        <v>188</v>
+      </c>
+      <c s="34" r="E10" t="s">
+        <v>187</v>
+      </c>
+      <c s="35" r="F10" t="s">
+        <v>188</v>
+      </c>
+      <c s="34" r="G10" t="s">
+        <v>187</v>
+      </c>
+      <c s="35" r="H10" t="s">
+        <v>188</v>
+      </c>
+      <c s="34" r="I10" t="s">
+        <v>187</v>
+      </c>
+      <c s="35" r="J10" t="s">
+        <v>188</v>
+      </c>
+      <c s="31" r="M10" t="s">
         <v>189</v>
       </c>
-      <c s="34" r="C10" t="s">
-        <v>188</v>
-      </c>
-      <c s="35" r="D10" t="s">
-        <v>189</v>
-      </c>
-      <c s="34" r="E10" t="s">
-        <v>188</v>
-      </c>
-      <c s="35" r="F10" t="s">
-        <v>189</v>
-      </c>
-      <c s="34" r="G10" t="s">
-        <v>188</v>
-      </c>
-      <c s="35" r="H10" t="s">
-        <v>189</v>
-      </c>
-      <c s="34" r="I10" t="s">
-        <v>188</v>
-      </c>
-      <c s="35" r="J10" t="s">
-        <v>189</v>
-      </c>
-      <c s="31" r="M10" t="s">
+      <c s="32" r="N10" t="s">
         <v>190</v>
-      </c>
-      <c s="32" r="N10" t="s">
-        <v>191</v>
       </c>
     </row>
     <row s="55" r="11" spans="1:20">
@@ -5354,7 +5335,7 @@
         <v>-7.616225854e-07</v>
       </c>
       <c r="M16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row s="55" r="17" spans="1:20">
@@ -5495,11 +5476,11 @@
       </c>
     </row>
     <row s="55" r="22" spans="1:20">
-      <c s="43" r="A22" t="s">
+      <c s="57" r="A22" t="s">
         <v>19</v>
       </c>
-      <c s="43" r="B22" t="s">
-        <v>193</v>
+      <c s="57" r="B22" t="s">
+        <v>154</v>
       </c>
     </row>
     <row s="55" r="23" spans="1:20">
@@ -5507,21 +5488,22 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="M23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row s="55" r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>194</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="B24" t="s"/>
       <c r="C24" t="s">
+        <v>181</v>
+      </c>
+      <c r="D24" t="s">
         <v>182</v>
-      </c>
-      <c r="D24" t="s">
-        <v>183</v>
       </c>
       <c r="M24" t="n">
         <v>1.098901098901099e-08</v>
@@ -5529,10 +5511,10 @@
     </row>
     <row s="55" r="25" spans="1:20">
       <c r="A25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C25" t="n">
         <v>1000000000</v>
@@ -5543,86 +5525,86 @@
     </row>
     <row s="55" r="26" spans="1:20">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B26" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C26" t="n">
-        <v>1000000</v>
+        <v>100000000</v>
       </c>
       <c r="D26" t="n">
         <v>1</v>
       </c>
     </row>
     <row s="55" r="27" spans="1:20">
-      <c s="50" r="A27" t="s">
+      <c s="64" r="A27" t="s">
+        <v>187</v>
+      </c>
+      <c s="65" r="B27" t="s">
         <v>188</v>
       </c>
-      <c s="51" r="B27" t="s">
+      <c s="64" r="C27" t="s">
+        <v>187</v>
+      </c>
+      <c s="65" r="D27" t="s">
+        <v>188</v>
+      </c>
+      <c s="64" r="E27" t="s">
+        <v>187</v>
+      </c>
+      <c s="65" r="F27" t="s">
+        <v>188</v>
+      </c>
+      <c s="64" r="G27" t="s">
+        <v>187</v>
+      </c>
+      <c s="65" r="H27" t="s">
+        <v>188</v>
+      </c>
+      <c s="64" r="I27" t="s">
+        <v>187</v>
+      </c>
+      <c s="65" r="J27" t="s">
+        <v>188</v>
+      </c>
+      <c s="31" r="M27" t="s">
         <v>189</v>
       </c>
-      <c s="50" r="C27" t="s">
-        <v>188</v>
-      </c>
-      <c s="51" r="D27" t="s">
-        <v>189</v>
-      </c>
-      <c s="50" r="E27" t="s">
-        <v>188</v>
-      </c>
-      <c s="51" r="F27" t="s">
-        <v>189</v>
-      </c>
-      <c s="50" r="G27" t="s">
-        <v>188</v>
-      </c>
-      <c s="51" r="H27" t="s">
-        <v>189</v>
-      </c>
-      <c s="50" r="I27" t="s">
-        <v>188</v>
-      </c>
-      <c s="51" r="J27" t="s">
-        <v>189</v>
-      </c>
-      <c s="31" r="M27" t="s">
+      <c s="32" r="N27" t="s">
         <v>190</v>
       </c>
-      <c s="32" r="N27" t="s">
-        <v>191</v>
-      </c>
     </row>
     <row s="55" r="28" spans="1:20">
-      <c s="50" r="A28" t="n">
-        <v>1.104339364600259e-05</v>
-      </c>
-      <c s="51" r="B28" t="n">
-        <v>-1.102052070415042e-05</v>
-      </c>
-      <c s="50" r="C28" t="n">
-        <v>1.112083556749776e-05</v>
-      </c>
-      <c s="51" r="D28" t="n">
-        <v>-1.100499099685229e-05</v>
-      </c>
-      <c s="50" r="E28" t="n">
-        <v>1.088810912802895e-05</v>
-      </c>
-      <c s="51" r="F28" t="n">
-        <v>-1.112776110868055e-05</v>
-      </c>
-      <c s="50" r="G28" t="n">
-        <v>1.11032541211641e-05</v>
-      </c>
-      <c s="51" r="H28" t="n">
-        <v>-1.086542222990888e-05</v>
-      </c>
-      <c s="50" r="I28" t="n">
-        <v>1.106458368829284e-05</v>
-      </c>
-      <c s="51" r="J28" t="n">
-        <v>-1.076520410473305e-05</v>
+      <c s="64" r="A28" t="n">
+        <v>1.111128859286232e-05</v>
+      </c>
+      <c s="65" r="B28" t="n">
+        <v>-1.082116919870992e-05</v>
+      </c>
+      <c s="64" r="C28" t="n">
+        <v>1.098525836429284e-05</v>
+      </c>
+      <c s="65" r="D28" t="n">
+        <v>-1.09035139525499e-05</v>
+      </c>
+      <c s="64" r="E28" t="n">
+        <v>1.101326724166088e-05</v>
+      </c>
+      <c s="65" r="F28" t="n">
+        <v>-1.105174063593678e-05</v>
+      </c>
+      <c s="64" r="G28" t="n">
+        <v>1.104213279602983e-05</v>
+      </c>
+      <c s="65" r="H28" t="n">
+        <v>-1.093497780098531e-05</v>
+      </c>
+      <c s="64" r="I28" t="n">
+        <v>1.102514660325083e-05</v>
+      </c>
+      <c s="65" r="J28" t="n">
+        <v>-1.075079247191027e-05</v>
       </c>
       <c r="M28" t="n">
         <v>-2.425690619522e-08</v>
@@ -5632,35 +5614,35 @@
       </c>
     </row>
     <row s="55" r="29" spans="1:20">
-      <c s="50" r="A29" t="n">
-        <v>1.101994097989272e-05</v>
-      </c>
-      <c s="51" r="B29" t="n">
-        <v>-1.111237827202198e-05</v>
-      </c>
-      <c s="50" r="C29" t="n">
-        <v>1.10985765161526e-05</v>
-      </c>
-      <c s="51" r="D29" t="n">
-        <v>-1.081162580367737e-05</v>
-      </c>
-      <c s="50" r="E29" t="n">
-        <v>1.116652664629528e-05</v>
-      </c>
-      <c s="51" r="F29" t="n">
-        <v>-1.112561901581021e-05</v>
-      </c>
-      <c s="50" r="G29" t="n">
-        <v>1.082587786046952e-05</v>
-      </c>
-      <c s="51" r="H29" t="n">
-        <v>-1.088118491272897e-05</v>
-      </c>
-      <c s="50" r="I29" t="n">
-        <v>1.101428126165593e-05</v>
-      </c>
-      <c s="51" r="J29" t="n">
-        <v>-1.095549976758487e-05</v>
+      <c s="64" r="A29" t="n">
+        <v>1.090022827529212e-05</v>
+      </c>
+      <c s="65" r="B29" t="n">
+        <v>-1.101370041098007e-05</v>
+      </c>
+      <c s="64" r="C29" t="n">
+        <v>1.093030989956194e-05</v>
+      </c>
+      <c s="65" r="D29" t="n">
+        <v>-1.084989685587355e-05</v>
+      </c>
+      <c s="64" r="E29" t="n">
+        <v>1.092396552237727e-05</v>
+      </c>
+      <c s="65" r="F29" t="n">
+        <v>-1.104211784586657e-05</v>
+      </c>
+      <c s="64" r="G29" t="n">
+        <v>1.080413856292303e-05</v>
+      </c>
+      <c s="65" r="H29" t="n">
+        <v>-1.10368989504856e-05</v>
+      </c>
+      <c s="64" r="I29" t="n">
+        <v>1.097551790063789e-05</v>
+      </c>
+      <c s="65" r="J29" t="n">
+        <v>-1.085137443174699e-05</v>
       </c>
       <c r="M29" t="n">
         <v>3.918342267654493e-07</v>
@@ -5670,35 +5652,35 @@
       </c>
     </row>
     <row s="55" r="30" spans="1:20">
-      <c s="50" r="A30" t="n">
-        <v>1.097740949696193e-05</v>
-      </c>
-      <c s="51" r="B30" t="n">
-        <v>-1.089798910676023e-05</v>
-      </c>
-      <c s="50" r="C30" t="n">
-        <v>1.099208295054066e-05</v>
-      </c>
-      <c s="51" r="D30" t="n">
-        <v>-1.107443930614636e-05</v>
-      </c>
-      <c s="50" r="E30" t="n">
-        <v>1.088735597116857e-05</v>
-      </c>
-      <c s="51" r="F30" t="n">
-        <v>-1.104089827892274e-05</v>
-      </c>
-      <c s="50" r="G30" t="n">
-        <v>1.087738676799388e-05</v>
-      </c>
-      <c s="51" r="H30" t="n">
-        <v>-1.102603651397573e-05</v>
-      </c>
-      <c s="50" r="I30" t="n">
-        <v>1.090874655083734e-05</v>
-      </c>
-      <c s="51" r="J30" t="n">
-        <v>-1.108868791149381e-05</v>
+      <c s="64" r="A30" t="n">
+        <v>1.114365755711997e-05</v>
+      </c>
+      <c s="65" r="B30" t="n">
+        <v>-1.118195662129844e-05</v>
+      </c>
+      <c s="64" r="C30" t="n">
+        <v>1.082455854105116e-05</v>
+      </c>
+      <c s="65" r="D30" t="n">
+        <v>-1.089905952099539e-05</v>
+      </c>
+      <c s="64" r="E30" t="n">
+        <v>1.133039500193132e-05</v>
+      </c>
+      <c s="65" r="F30" t="n">
+        <v>-1.114848699923234e-05</v>
+      </c>
+      <c s="64" r="G30" t="n">
+        <v>1.108133716586929e-05</v>
+      </c>
+      <c s="65" r="H30" t="n">
+        <v>-1.095964532131547e-05</v>
+      </c>
+      <c s="64" r="I30" t="n">
+        <v>1.107798600831523e-05</v>
+      </c>
+      <c s="65" r="J30" t="n">
+        <v>-1.097335996979085e-05</v>
       </c>
       <c r="M30" t="n">
         <v>49</v>
@@ -5708,279 +5690,279 @@
       </c>
     </row>
     <row s="55" r="31" spans="1:20">
-      <c s="50" r="A31" t="n">
-        <v>1.109707774070863e-05</v>
-      </c>
-      <c s="51" r="B31" t="n">
-        <v>-1.120484239569209e-05</v>
-      </c>
-      <c s="50" r="C31" t="n">
-        <v>1.115032030954542e-05</v>
-      </c>
-      <c s="51" r="D31" t="n">
-        <v>-1.100834788708769e-05</v>
-      </c>
-      <c s="50" r="E31" t="n">
-        <v>1.102329192566298e-05</v>
-      </c>
-      <c s="51" r="F31" t="n">
-        <v>-1.098898947259973e-05</v>
-      </c>
-      <c s="50" r="G31" t="n">
-        <v>1.099873415976007e-05</v>
-      </c>
-      <c s="51" r="H31" t="n">
-        <v>-1.105951806648551e-05</v>
-      </c>
-      <c s="50" r="I31" t="n">
-        <v>1.087671076848252e-05</v>
-      </c>
-      <c s="51" r="J31" t="n">
-        <v>-1.102197912650231e-05</v>
+      <c s="64" r="A31" t="n">
+        <v>1.09273618799371e-05</v>
+      </c>
+      <c s="65" r="B31" t="n">
+        <v>-1.08510452264633e-05</v>
+      </c>
+      <c s="64" r="C31" t="n">
+        <v>1.107627184758177e-05</v>
+      </c>
+      <c s="65" r="D31" t="n">
+        <v>-1.103144169337835e-05</v>
+      </c>
+      <c s="64" r="E31" t="n">
+        <v>1.108028659670026e-05</v>
+      </c>
+      <c s="65" r="F31" t="n">
+        <v>-1.085760882699556e-05</v>
+      </c>
+      <c s="64" r="G31" t="n">
+        <v>1.118592470950626e-05</v>
+      </c>
+      <c s="65" r="H31" t="n">
+        <v>-1.099289792959733e-05</v>
+      </c>
+      <c s="64" r="I31" t="n">
+        <v>1.09439357196777e-05</v>
+      </c>
+      <c s="65" r="J31" t="n">
+        <v>-1.110021243723675e-05</v>
       </c>
     </row>
     <row s="55" r="32" spans="1:20">
-      <c s="50" r="A32" t="n">
-        <v>1.130386744905342e-05</v>
-      </c>
-      <c s="51" r="B32" t="n">
-        <v>-1.109359498141882e-05</v>
-      </c>
-      <c s="50" r="C32" t="n">
-        <v>1.098332096732271e-05</v>
-      </c>
-      <c s="51" r="D32" t="n">
-        <v>-1.103137448566092e-05</v>
-      </c>
-      <c s="50" r="E32" t="n">
-        <v>1.096872578388309e-05</v>
-      </c>
-      <c s="51" r="F32" t="n">
-        <v>-1.085632459569711e-05</v>
-      </c>
-      <c s="50" r="G32" t="n">
-        <v>1.105319855650008e-05</v>
-      </c>
-      <c s="51" r="H32" t="n">
-        <v>-1.094874997546479e-05</v>
-      </c>
-      <c s="50" r="I32" t="n">
-        <v>1.103021386597666e-05</v>
-      </c>
-      <c s="51" r="J32" t="n">
-        <v>-1.103376869795102e-05</v>
+      <c s="64" r="A32" t="n">
+        <v>1.109944901463142e-05</v>
+      </c>
+      <c s="65" r="B32" t="n">
+        <v>-1.094063929735949e-05</v>
+      </c>
+      <c s="64" r="C32" t="n">
+        <v>1.10509775638285e-05</v>
+      </c>
+      <c s="65" r="D32" t="n">
+        <v>-1.097338372130156e-05</v>
+      </c>
+      <c s="64" r="E32" t="n">
+        <v>1.099549397288064e-05</v>
+      </c>
+      <c s="65" r="F32" t="n">
+        <v>-1.095580941983887e-05</v>
+      </c>
+      <c s="64" r="G32" t="n">
+        <v>1.114814589748716e-05</v>
+      </c>
+      <c s="65" r="H32" t="n">
+        <v>-1.0988158947059e-05</v>
+      </c>
+      <c s="64" r="I32" t="n">
+        <v>1.106223371041575e-05</v>
+      </c>
+      <c s="65" r="J32" t="n">
+        <v>-1.099618096855123e-05</v>
       </c>
     </row>
     <row s="55" r="33" spans="1:20">
-      <c s="50" r="A33" t="n">
-        <v>1.072906822589163e-05</v>
-      </c>
-      <c s="51" r="B33" t="n">
-        <v>-1.098696579640201e-05</v>
-      </c>
-      <c s="50" r="C33" t="n">
-        <v>1.108029714199913e-05</v>
-      </c>
-      <c s="51" r="D33" t="n">
-        <v>-1.091045185691885e-05</v>
-      </c>
-      <c s="50" r="E33" t="n">
-        <v>1.099917428301678e-05</v>
-      </c>
-      <c s="51" r="F33" t="n">
-        <v>-1.097030494432233e-05</v>
-      </c>
-      <c s="50" r="G33" t="n">
-        <v>1.111109676818503e-05</v>
-      </c>
-      <c s="51" r="H33" t="n">
-        <v>-1.103944489565402e-05</v>
-      </c>
-      <c s="50" r="I33" t="n">
-        <v>1.099177321678114e-05</v>
-      </c>
-      <c s="51" r="J33" t="n">
-        <v>-1.092142980057622e-05</v>
+      <c s="64" r="A33" t="n">
+        <v>1.095184504759529e-05</v>
+      </c>
+      <c s="65" r="B33" t="n">
+        <v>-1.103561405455641e-05</v>
+      </c>
+      <c s="64" r="C33" t="n">
+        <v>1.090055488941644e-05</v>
+      </c>
+      <c s="65" r="D33" t="n">
+        <v>-1.092897232101499e-05</v>
+      </c>
+      <c s="64" r="E33" t="n">
+        <v>1.110323495682629e-05</v>
+      </c>
+      <c s="65" r="F33" t="n">
+        <v>-1.09840734545857e-05</v>
+      </c>
+      <c s="64" r="G33" t="n">
+        <v>1.103835419802977e-05</v>
+      </c>
+      <c s="65" r="H33" t="n">
+        <v>-1.101106173025462e-05</v>
+      </c>
+      <c s="64" r="I33" t="n">
+        <v>1.104169799328775e-05</v>
+      </c>
+      <c s="65" r="J33" t="n">
+        <v>-1.109291837425951e-05</v>
       </c>
       <c r="M33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row s="55" r="34" spans="1:20">
-      <c s="50" r="A34" t="n">
-        <v>1.102729202144005e-05</v>
-      </c>
-      <c s="51" r="B34" t="n">
-        <v>-1.102426261702664e-05</v>
-      </c>
-      <c s="50" r="C34" t="n">
-        <v>1.092362562813499e-05</v>
-      </c>
-      <c s="51" r="D34" t="n">
-        <v>-1.0867834872149e-05</v>
-      </c>
-      <c s="50" r="E34" t="n">
-        <v>1.097187707445251e-05</v>
-      </c>
-      <c s="51" r="F34" t="n">
-        <v>-1.103361430653677e-05</v>
-      </c>
-      <c s="50" r="G34" t="n">
-        <v>1.110937802233701e-05</v>
-      </c>
-      <c s="51" r="H34" t="n">
-        <v>-1.107201208170334e-05</v>
-      </c>
-      <c s="50" r="I34" t="n">
-        <v>1.091095438931515e-05</v>
-      </c>
-      <c s="51" r="J34" t="n">
-        <v>-1.079612549690955e-05</v>
+      <c s="64" r="A34" t="n">
+        <v>1.080600650973956e-05</v>
+      </c>
+      <c s="65" r="B34" t="n">
+        <v>-1.10586616913258e-05</v>
+      </c>
+      <c s="64" r="C34" t="n">
+        <v>1.099353450921344e-05</v>
+      </c>
+      <c s="65" r="D34" t="n">
+        <v>-1.083530604452111e-05</v>
+      </c>
+      <c s="64" r="E34" t="n">
+        <v>1.101848027158349e-05</v>
+      </c>
+      <c s="65" r="F34" t="n">
+        <v>-1.100958360428644e-05</v>
+      </c>
+      <c s="64" r="G34" t="n">
+        <v>1.108395065356388e-05</v>
+      </c>
+      <c s="65" r="H34" t="n">
+        <v>-1.095700720356318e-05</v>
+      </c>
+      <c s="64" r="I34" t="n">
+        <v>1.096872318691264e-05</v>
+      </c>
+      <c s="65" r="J34" t="n">
+        <v>-1.098516756844001e-05</v>
       </c>
       <c s="17" r="M34" t="n">
         <v>0.005117054126783899</v>
       </c>
     </row>
     <row s="55" r="35" spans="1:20">
-      <c s="50" r="A35" t="n">
-        <v>1.10257707090435e-05</v>
-      </c>
-      <c s="51" r="B35" t="n">
-        <v>-1.082753450186405e-05</v>
-      </c>
-      <c s="50" r="C35" t="n">
-        <v>1.096457397036158e-05</v>
-      </c>
-      <c s="51" r="D35" t="n">
-        <v>-1.103868008941529e-05</v>
-      </c>
-      <c s="50" r="E35" t="n">
-        <v>1.0990130088416e-05</v>
-      </c>
-      <c s="51" r="F35" t="n">
-        <v>-1.126867833701853e-05</v>
-      </c>
-      <c s="50" r="G35" t="n">
-        <v>1.096087298799423e-05</v>
-      </c>
-      <c s="51" r="H35" t="n">
-        <v>-1.104556803069215e-05</v>
-      </c>
-      <c s="50" r="I35" t="n">
-        <v>1.087707801733295e-05</v>
-      </c>
-      <c s="51" r="J35" t="n">
-        <v>-1.112257504980168e-05</v>
+      <c s="64" r="A35" t="n">
+        <v>1.113748279023496e-05</v>
+      </c>
+      <c s="65" r="B35" t="n">
+        <v>-1.093302717104113e-05</v>
+      </c>
+      <c s="64" r="C35" t="n">
+        <v>1.096409239254451e-05</v>
+      </c>
+      <c s="65" r="D35" t="n">
+        <v>-1.094866235568759e-05</v>
+      </c>
+      <c s="64" r="E35" t="n">
+        <v>1.076193881401705e-05</v>
+      </c>
+      <c s="65" r="F35" t="n">
+        <v>-1.094247744538984e-05</v>
+      </c>
+      <c s="64" r="G35" t="n">
+        <v>1.096900654631768e-05</v>
+      </c>
+      <c s="65" r="H35" t="n">
+        <v>-1.098343029814674e-05</v>
+      </c>
+      <c s="64" r="I35" t="n">
+        <v>1.11128274654694e-05</v>
+      </c>
+      <c s="65" r="J35" t="n">
+        <v>-1.091302322975078e-05</v>
       </c>
       <c s="17" r="M35" t="n">
         <v>0.002937060600972517</v>
       </c>
     </row>
     <row s="55" r="36" spans="1:20">
-      <c s="50" r="A36" t="n">
-        <v>1.098998586510615e-05</v>
-      </c>
-      <c s="51" r="B36" t="n">
-        <v>-1.091940424336834e-05</v>
-      </c>
-      <c s="50" r="C36" t="n">
-        <v>1.122376583436084e-05</v>
-      </c>
-      <c s="51" r="D36" t="n">
-        <v>-1.114650239088899e-05</v>
-      </c>
-      <c s="50" r="E36" t="n">
-        <v>1.104640130578588e-05</v>
-      </c>
-      <c s="51" r="F36" t="n">
-        <v>-1.100143580119379e-05</v>
-      </c>
-      <c s="50" r="G36" t="n">
-        <v>1.082693558274751e-05</v>
-      </c>
-      <c s="51" r="H36" t="n">
-        <v>-1.108594670118507e-05</v>
-      </c>
-      <c s="50" r="I36" t="n">
-        <v>1.091466201669468e-05</v>
-      </c>
-      <c s="51" r="J36" t="n">
-        <v>-1.094182299569284e-05</v>
+      <c s="64" r="A36" t="n">
+        <v>1.105701083195259e-05</v>
+      </c>
+      <c s="65" r="B36" t="n">
+        <v>-1.108936608070832e-05</v>
+      </c>
+      <c s="64" r="C36" t="n">
+        <v>1.098601134565646e-05</v>
+      </c>
+      <c s="65" r="D36" t="n">
+        <v>-1.095107357215492e-05</v>
+      </c>
+      <c s="64" r="E36" t="n">
+        <v>1.092238955391944e-05</v>
+      </c>
+      <c s="65" r="F36" t="n">
+        <v>-1.084051209490265e-05</v>
+      </c>
+      <c s="64" r="G36" t="n">
+        <v>1.110903496829714e-05</v>
+      </c>
+      <c s="65" r="H36" t="n">
+        <v>-1.110917761359627e-05</v>
+      </c>
+      <c s="64" r="I36" t="n">
+        <v>1.094682613510683e-05</v>
+      </c>
+      <c s="65" r="J36" t="n">
+        <v>-1.106197235225377e-05</v>
       </c>
       <c s="12" r="M36" t="n">
         <v>96.82660421439783</v>
       </c>
     </row>
     <row s="55" r="37" spans="1:20">
-      <c s="50" r="A37" t="n">
-        <v>1.070304779318875e-05</v>
-      </c>
-      <c s="51" r="B37" t="n">
-        <v>-1.100093917513632e-05</v>
-      </c>
-      <c s="50" r="C37" t="n">
-        <v>1.103379033859362e-05</v>
-      </c>
-      <c s="51" r="D37" t="n">
-        <v>-1.111127637946324e-05</v>
-      </c>
-      <c s="50" r="E37" t="n">
-        <v>1.09079267148041e-05</v>
-      </c>
-      <c s="51" r="F37" t="n">
-        <v>-1.099005227698923e-05</v>
-      </c>
-      <c s="50" r="G37" t="n">
-        <v>1.093715426870302e-05</v>
-      </c>
-      <c s="51" r="H37" t="n">
-        <v>-1.097905991880286e-05</v>
-      </c>
-      <c s="50" r="I37" t="n">
-        <v>1.109043500030451e-05</v>
-      </c>
-      <c s="51" r="J37" t="n">
-        <v>-1.101367545402407e-05</v>
+      <c s="64" r="A37" t="n">
+        <v>1.110993332867541e-05</v>
+      </c>
+      <c s="65" r="B37" t="n">
+        <v>-1.103518008405607e-05</v>
+      </c>
+      <c s="64" r="C37" t="n">
+        <v>1.093950028276945e-05</v>
+      </c>
+      <c s="65" r="D37" t="n">
+        <v>-1.102272546800555e-05</v>
+      </c>
+      <c s="64" r="E37" t="n">
+        <v>1.095678694192023e-05</v>
+      </c>
+      <c s="65" r="F37" t="n">
+        <v>-1.099369366169114e-05</v>
+      </c>
+      <c s="64" r="G37" t="n">
+        <v>1.107195443963907e-05</v>
+      </c>
+      <c s="65" r="H37" t="n">
+        <v>-1.110295615199901e-05</v>
+      </c>
+      <c s="64" r="I37" t="n">
+        <v>1.105546130281027e-05</v>
+      </c>
+      <c s="65" r="J37" t="n">
+        <v>-1.11236951194603e-05</v>
       </c>
     </row>
     <row s="55" r="180" spans="1:20">
       <c r="O180" t="s">
+        <v>187</v>
+      </c>
+      <c r="P180" t="s">
         <v>188</v>
       </c>
-      <c r="P180" t="s">
-        <v>189</v>
-      </c>
       <c r="Q180" t="s">
+        <v>187</v>
+      </c>
+      <c r="R180" t="s">
         <v>188</v>
       </c>
-      <c r="R180" t="s">
-        <v>189</v>
-      </c>
       <c r="S180" t="s">
+        <v>187</v>
+      </c>
+      <c r="T180" t="s">
         <v>188</v>
-      </c>
-      <c r="T180" t="s">
-        <v>189</v>
       </c>
     </row>
     <row s="55" r="197" spans="1:20">
       <c r="O197" t="s">
+        <v>187</v>
+      </c>
+      <c r="P197" t="s">
         <v>188</v>
       </c>
-      <c r="P197" t="s">
-        <v>189</v>
-      </c>
       <c r="Q197" t="s">
+        <v>187</v>
+      </c>
+      <c r="R197" t="s">
         <v>188</v>
       </c>
-      <c r="R197" t="s">
-        <v>189</v>
-      </c>
       <c r="S197" t="s">
+        <v>187</v>
+      </c>
+      <c r="T197" t="s">
         <v>188</v>
-      </c>
-      <c r="T197" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -6022,77 +6004,77 @@
     <col bestFit="1" customWidth="1" max="14" min="14" style="55" width="23.28515625"/>
     <col customWidth="1" max="15" min="15" style="55" width="74"/>
     <col customWidth="1" max="16" min="16" style="55" width="11.42578125"/>
-    <col customWidth="1" hidden="1" max="21" min="17" style="55"/>
-    <col customWidth="1" hidden="1" max="21" min="17" style="55"/>
-    <col customWidth="1" hidden="1" max="21" min="17" style="55"/>
-    <col customWidth="1" hidden="1" max="21" min="17" style="55"/>
-    <col customWidth="1" hidden="1" max="21" min="17" style="55"/>
+    <col hidden="1" max="21" min="17" style="55"/>
+    <col hidden="1" max="21" min="17" style="55"/>
+    <col hidden="1" max="21" min="17" style="55"/>
+    <col hidden="1" max="21" min="17" style="55"/>
+    <col hidden="1" max="21" min="17" style="55"/>
   </cols>
   <sheetData>
     <row s="55" r="1" spans="1:21">
       <c s="7" r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c s="7" r="I1" t="s">
+        <v>196</v>
+      </c>
+      <c s="37" r="Q1" t="s">
         <v>197</v>
-      </c>
-      <c s="7" r="I1" t="s">
-        <v>198</v>
-      </c>
-      <c s="37" r="Q1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row s="55" r="2" spans="1:21">
       <c s="14" r="A2" t="s">
+        <v>198</v>
+      </c>
+      <c s="14" r="B2" t="s">
+        <v>199</v>
+      </c>
+      <c s="14" r="C2" t="s">
         <v>200</v>
       </c>
-      <c s="14" r="B2" t="s">
+      <c s="14" r="D2" t="s">
         <v>201</v>
       </c>
-      <c s="14" r="C2" t="s">
+      <c s="14" r="E2" t="s">
         <v>202</v>
       </c>
-      <c s="14" r="D2" t="s">
+      <c s="14" r="F2" t="s">
         <v>203</v>
       </c>
-      <c s="14" r="E2" t="s">
+      <c s="36" r="G2" t="s">
         <v>204</v>
       </c>
-      <c s="14" r="F2" t="s">
+      <c s="14" r="I2" t="s">
+        <v>198</v>
+      </c>
+      <c s="14" r="J2" t="s">
+        <v>199</v>
+      </c>
+      <c s="14" r="K2" t="s">
+        <v>200</v>
+      </c>
+      <c s="14" r="L2" t="s">
+        <v>201</v>
+      </c>
+      <c s="14" r="M2" t="s">
+        <v>202</v>
+      </c>
+      <c s="14" r="N2" t="s">
+        <v>203</v>
+      </c>
+      <c s="36" r="O2" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q2" t="s">
         <v>205</v>
-      </c>
-      <c s="36" r="G2" t="s">
-        <v>206</v>
-      </c>
-      <c s="14" r="I2" t="s">
-        <v>200</v>
-      </c>
-      <c s="14" r="J2" t="s">
-        <v>201</v>
-      </c>
-      <c s="14" r="K2" t="s">
-        <v>202</v>
-      </c>
-      <c s="14" r="L2" t="s">
-        <v>203</v>
-      </c>
-      <c s="14" r="M2" t="s">
-        <v>204</v>
-      </c>
-      <c s="14" r="N2" t="s">
-        <v>205</v>
-      </c>
-      <c s="36" r="O2" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row s="55" r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C3" t="n">
         <v>100.0118</v>
@@ -6101,36 +6083,36 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" t="s">
+        <v>209</v>
+      </c>
+      <c s="40" r="G3" t="s">
         <v>210</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J3" t="s">
         <v>211</v>
       </c>
-      <c s="40" r="G3" t="s">
+      <c r="N3" t="s">
         <v>212</v>
       </c>
-      <c r="I3" t="s">
-        <v>174</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="O3" t="s">
         <v>213</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>214</v>
-      </c>
-      <c r="O3" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>216</v>
       </c>
     </row>
     <row s="55" r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -6139,33 +6121,33 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F4" t="s">
+        <v>216</v>
+      </c>
+      <c r="I4" t="s">
+        <v>173</v>
+      </c>
+      <c r="J4" t="s">
+        <v>217</v>
+      </c>
+      <c r="N4" t="s">
         <v>218</v>
       </c>
-      <c r="I4" t="s">
-        <v>174</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="O4" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q4" t="s">
         <v>219</v>
-      </c>
-      <c r="N4" t="s">
-        <v>220</v>
-      </c>
-      <c r="O4" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>221</v>
       </c>
     </row>
     <row s="55" r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c s="21" r="C5" t="n">
         <v>0.00390912</v>
@@ -6174,33 +6156,33 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F5" t="s">
+        <v>221</v>
+      </c>
+      <c r="I5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J5" t="s">
+        <v>222</v>
+      </c>
+      <c r="N5" t="s">
         <v>223</v>
       </c>
-      <c r="I5" t="s">
-        <v>174</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="O5" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q5" t="s">
         <v>224</v>
-      </c>
-      <c r="N5" t="s">
-        <v>225</v>
-      </c>
-      <c r="O5" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>226</v>
       </c>
     </row>
     <row s="55" r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c s="21" r="C6" t="n">
         <v>-5.926000000000001e-07</v>
@@ -6209,59 +6191,59 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K6" t="n">
         <v>6</v>
       </c>
       <c r="O6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="Q6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row s="55" r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c s="22" r="C7" t="n">
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J7" t="s">
+        <v>231</v>
+      </c>
+      <c r="K7" t="s">
+        <v>232</v>
+      </c>
+      <c r="O7" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q7" t="s">
         <v>233</v>
-      </c>
-      <c r="K7" t="s">
-        <v>234</v>
-      </c>
-      <c r="O7" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>235</v>
       </c>
     </row>
     <row s="55" r="8" spans="1:21">
       <c s="14" r="A8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c s="14" r="B8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c s="14" r="C8" t="s">
         <v>37</v>
@@ -6271,24 +6253,24 @@
       <c s="14" r="F8" t="n"/>
       <c s="36" r="G8" t="n"/>
       <c r="I8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J8" t="s">
+        <v>235</v>
+      </c>
+      <c r="K8" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q8" t="s">
         <v>237</v>
-      </c>
-      <c r="K8" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>239</v>
       </c>
     </row>
     <row s="55" r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c s="21" r="C9" t="n">
         <v>10000.2</v>
@@ -6297,34 +6279,34 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F9" t="s">
+        <v>239</v>
+      </c>
+      <c s="36" r="I9" t="s">
+        <v>173</v>
+      </c>
+      <c s="36" r="J9" t="s">
+        <v>240</v>
+      </c>
+      <c s="36" r="K9" t="s">
         <v>241</v>
-      </c>
-      <c s="36" r="I9" t="s">
-        <v>174</v>
-      </c>
-      <c s="36" r="J9" t="s">
-        <v>242</v>
-      </c>
-      <c s="36" r="K9" t="s">
-        <v>243</v>
       </c>
       <c s="36" r="L9" t="n"/>
       <c s="36" r="M9" t="n"/>
       <c s="36" r="N9" t="n"/>
       <c s="36" r="O9" t="n"/>
       <c r="Q9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row s="55" r="10" spans="1:21">
       <c r="A10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c s="21" r="C10" t="n">
         <v>23</v>
@@ -6333,16 +6315,16 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F10" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c s="21" r="K10" t="n">
         <v>-0.001</v>
@@ -6351,24 +6333,24 @@
         <v>0.00045</v>
       </c>
       <c r="M10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c s="37" r="R10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row s="55" r="11" spans="1:21">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c s="21" r="C11" t="n">
         <v>0.001</v>
@@ -6377,36 +6359,36 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K11" t="n">
         <v>5</v>
       </c>
       <c r="O11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="R11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c s="37" r="S11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row s="55" r="12" spans="1:21">
       <c r="A12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c s="21" r="C12" t="n">
         <v>0</v>
@@ -6415,62 +6397,62 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F12" t="s">
+        <v>249</v>
+      </c>
+      <c r="I12" t="s">
+        <v>169</v>
+      </c>
+      <c r="J12" t="s">
+        <v>231</v>
+      </c>
+      <c r="K12" t="s">
+        <v>250</v>
+      </c>
+      <c r="O12" t="s">
+        <v>228</v>
+      </c>
+      <c r="S12" t="s">
         <v>251</v>
       </c>
-      <c r="I12" t="s">
-        <v>170</v>
-      </c>
-      <c r="J12" t="s">
-        <v>233</v>
-      </c>
-      <c r="K12" t="s">
+      <c s="37" r="T12" t="s">
         <v>252</v>
-      </c>
-      <c r="O12" t="s">
-        <v>230</v>
-      </c>
-      <c r="S12" t="s">
-        <v>253</v>
-      </c>
-      <c s="37" r="T12" t="s">
-        <v>254</v>
       </c>
     </row>
     <row s="55" r="13" spans="1:21">
       <c r="A13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c s="22" r="C13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K13" t="s">
+        <v>253</v>
+      </c>
+      <c r="T13" t="s">
+        <v>254</v>
+      </c>
+      <c s="37" r="U13" t="s">
         <v>255</v>
-      </c>
-      <c r="T13" t="s">
-        <v>256</v>
-      </c>
-      <c s="37" r="U13" t="s">
-        <v>257</v>
       </c>
     </row>
     <row s="55" r="14" spans="1:21">
       <c s="14" r="A14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c s="14" r="B14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c s="14" r="C14" t="s">
         <v>37</v>
@@ -6480,10 +6462,10 @@
       <c s="14" r="F14" t="n"/>
       <c s="36" r="G14" t="n"/>
       <c s="36" r="I14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c s="36" r="J14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K14" t="s">
         <v>24</v>
@@ -6492,18 +6474,18 @@
       <c s="36" r="M14" t="n"/>
       <c s="36" r="N14" t="n"/>
       <c s="36" r="O14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c s="37" r="T14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row s="55" r="15" spans="1:21">
       <c r="A15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C15" t="n">
         <v>9999.999260000001</v>
@@ -6515,13 +6497,13 @@
         <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c s="21" r="K15" t="n">
         <v>-0.0005</v>
@@ -6530,25 +6512,25 @@
         <v>0.0004</v>
       </c>
       <c r="M15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N15" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="O15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c s="37" r="S15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c s="37" r="T15" t="n"/>
     </row>
     <row s="55" r="16" spans="1:21">
       <c r="A16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c s="10" r="C16" t="n">
         <v>20</v>
@@ -6557,34 +6539,34 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K16" t="n">
         <v>4</v>
       </c>
       <c r="O16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c s="37" r="S16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c s="37" r="T16" t="n"/>
     </row>
     <row s="55" r="17" spans="1:21">
       <c r="A17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B17" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c s="21" r="C17" t="n">
         <v>5</v>
@@ -6593,34 +6575,34 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F17" t="s">
+        <v>264</v>
+      </c>
+      <c r="I17" t="s">
+        <v>170</v>
+      </c>
+      <c r="J17" t="s">
+        <v>231</v>
+      </c>
+      <c r="K17" t="s">
+        <v>265</v>
+      </c>
+      <c r="O17" t="s">
+        <v>228</v>
+      </c>
+      <c s="37" r="S17" t="s">
         <v>266</v>
-      </c>
-      <c r="I17" t="s">
-        <v>171</v>
-      </c>
-      <c r="J17" t="s">
-        <v>233</v>
-      </c>
-      <c r="K17" t="s">
-        <v>267</v>
-      </c>
-      <c r="O17" t="s">
-        <v>230</v>
-      </c>
-      <c s="37" r="S17" t="s">
-        <v>268</v>
       </c>
       <c s="37" r="T17" t="n"/>
     </row>
     <row s="55" r="18" spans="1:21">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B18" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C18" t="n">
         <v>9999.999260000001</v>
@@ -6632,30 +6614,30 @@
         <v>16</v>
       </c>
       <c r="F18" t="s">
+        <v>268</v>
+      </c>
+      <c r="I18" t="s">
+        <v>170</v>
+      </c>
+      <c r="J18" t="s">
+        <v>235</v>
+      </c>
+      <c r="K18" t="s">
+        <v>269</v>
+      </c>
+      <c r="S18" t="s">
+        <v>251</v>
+      </c>
+      <c r="T18" t="s">
         <v>270</v>
-      </c>
-      <c r="I18" t="s">
-        <v>171</v>
-      </c>
-      <c r="J18" t="s">
-        <v>237</v>
-      </c>
-      <c r="K18" t="s">
-        <v>271</v>
-      </c>
-      <c r="S18" t="s">
-        <v>253</v>
-      </c>
-      <c r="T18" t="s">
-        <v>272</v>
       </c>
     </row>
     <row s="55" r="19" spans="1:21">
       <c r="A19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B19" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c s="10" r="C19" t="n">
         <v>20</v>
@@ -6664,16 +6646,16 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F19" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c s="36" r="I19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c s="36" r="J19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K19" t="s">
         <v>24</v>
@@ -6682,18 +6664,18 @@
       <c s="36" r="M19" t="n"/>
       <c s="36" r="N19" t="n"/>
       <c s="36" r="O19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="T19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row s="55" r="20" spans="1:21">
       <c r="A20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B20" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C20" t="n">
         <v>10</v>
@@ -6702,30 +6684,30 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F20" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I20" t="s">
         <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K20" t="n">
         <v>2</v>
       </c>
       <c s="37" r="S20" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row s="55" r="21" spans="1:21">
       <c r="A21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c s="21" r="C21" t="n">
         <v>3.42e-07</v>
@@ -6737,30 +6719,30 @@
         <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I21" t="s">
         <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="S21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="T21" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row s="55" r="22" spans="1:21">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B22" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c s="21" r="C22" t="n">
         <v>-2.7e-08</v>
@@ -6772,27 +6754,27 @@
         <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I22" t="s">
         <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K22" t="s">
         <v>66</v>
       </c>
       <c r="T22" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row s="55" r="23" spans="1:21">
       <c r="A23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B23" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -6801,37 +6783,37 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c s="36" r="I23" t="s">
         <v>10</v>
       </c>
       <c s="36" r="J23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K23" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c s="36" r="L23" t="n"/>
       <c s="36" r="M23" t="n"/>
       <c s="36" r="N23" t="n"/>
       <c s="36" r="O23" t="n"/>
       <c r="T23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="U23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row s="55" r="24" spans="1:21">
       <c r="A24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B24" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c s="22" r="C24" t="n">
         <v>42522</v>
@@ -6840,7 +6822,7 @@
         <v>9</v>
       </c>
       <c r="J24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K24" t="n">
         <v>2</v>
@@ -6848,13 +6830,13 @@
     </row>
     <row s="55" r="25" spans="1:21">
       <c s="14" r="A25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c s="14" r="B25" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c s="14" r="C25" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c s="14" r="D25" t="n"/>
       <c s="14" r="E25" t="n"/>
@@ -6864,10 +6846,10 @@
         <v>9</v>
       </c>
       <c r="J25" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K25" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row s="55" r="26" spans="1:21">
@@ -6875,7 +6857,7 @@
         <v>9</v>
       </c>
       <c r="J26" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K26" t="s">
         <v>66</v>
@@ -6886,18 +6868,18 @@
         <v>9</v>
       </c>
       <c r="J27" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K27" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row s="55" r="28" spans="1:21">
       <c s="13" r="I28" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c s="13" r="J28" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c s="13" r="K28" t="n">
         <v>2</v>
@@ -6909,21 +6891,21 @@
     </row>
     <row s="55" r="29" spans="1:21">
       <c r="I29" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J29" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K29" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row s="55" r="30" spans="1:21">
       <c r="I30" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K30" t="s">
         <v>66</v>
@@ -6931,13 +6913,13 @@
     </row>
     <row s="55" r="31" spans="1:21">
       <c s="36" r="I31" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c s="36" r="J31" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K31" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c s="36" r="L31" t="n"/>
       <c s="36" r="M31" t="n"/>
@@ -6949,7 +6931,7 @@
         <v>8</v>
       </c>
       <c r="J32" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K32" t="n">
         <v>2</v>
@@ -6960,10 +6942,10 @@
         <v>8</v>
       </c>
       <c r="J33" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K33" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row s="55" r="34" spans="1:21">
@@ -6971,7 +6953,7 @@
         <v>8</v>
       </c>
       <c r="J34" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K34" t="s">
         <v>66</v>
@@ -6982,10 +6964,10 @@
         <v>8</v>
       </c>
       <c s="36" r="J35" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K35" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c s="36" r="L35" t="n"/>
       <c s="36" r="M35" t="n"/>
@@ -6997,7 +6979,7 @@
         <v>37</v>
       </c>
       <c r="J36" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K36" t="n">
         <v>0</v>
@@ -7006,7 +6988,7 @@
         <v>0</v>
       </c>
       <c r="M36" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="37" spans="1:21">
@@ -7014,7 +6996,7 @@
         <v>37</v>
       </c>
       <c r="J37" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K37" t="n">
         <v>0</v>
@@ -7023,7 +7005,7 @@
         <v>0</v>
       </c>
       <c r="M37" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="38" spans="1:21">
@@ -7031,7 +7013,7 @@
         <v>37</v>
       </c>
       <c r="J38" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K38" t="n">
         <v>0</v>
@@ -7040,7 +7022,7 @@
         <v>0</v>
       </c>
       <c r="M38" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="39" spans="1:21">
@@ -7048,7 +7030,7 @@
         <v>37</v>
       </c>
       <c r="J39" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K39" t="n">
         <v>0</v>
@@ -7057,7 +7039,7 @@
         <v>0</v>
       </c>
       <c r="M39" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="40" spans="1:21">
@@ -7065,7 +7047,7 @@
         <v>37</v>
       </c>
       <c r="J40" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K40" t="n">
         <v>0</v>
@@ -7074,7 +7056,7 @@
         <v>0</v>
       </c>
       <c r="M40" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="41" spans="1:21">
@@ -7082,7 +7064,7 @@
         <v>37</v>
       </c>
       <c r="J41" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K41" t="n">
         <v>0</v>
@@ -7091,7 +7073,7 @@
         <v>0</v>
       </c>
       <c r="M41" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="42" spans="1:21">
@@ -7099,7 +7081,7 @@
         <v>37</v>
       </c>
       <c r="J42" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K42" t="n">
         <v>0</v>
@@ -7108,7 +7090,7 @@
         <v>0</v>
       </c>
       <c r="M42" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="43" spans="1:21">
@@ -7116,7 +7098,7 @@
         <v>37</v>
       </c>
       <c r="J43" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K43" t="n">
         <v>0</v>
@@ -7125,7 +7107,7 @@
         <v>0</v>
       </c>
       <c r="M43" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="44" spans="1:21">
@@ -7133,7 +7115,7 @@
         <v>37</v>
       </c>
       <c r="J44" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K44" t="n">
         <v>0</v>
@@ -7144,10 +7126,10 @@
         <v>37</v>
       </c>
       <c r="J45" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K45" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row s="55" r="46" spans="1:21">
@@ -7155,10 +7137,10 @@
         <v>37</v>
       </c>
       <c r="J46" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K46" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row s="55" r="47" spans="1:21">
@@ -7166,7 +7148,7 @@
         <v>37</v>
       </c>
       <c s="36" r="J47" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K47" t="n"/>
       <c s="36" r="L47" t="n"/>
@@ -7176,10 +7158,10 @@
     </row>
     <row s="55" r="48" spans="1:21">
       <c r="I48" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J48" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K48" t="n">
         <v>0</v>
@@ -7188,15 +7170,15 @@
         <v>0</v>
       </c>
       <c r="M48" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="49" spans="1:21">
       <c r="I49" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J49" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K49" t="n">
         <v>0</v>
@@ -7205,15 +7187,15 @@
         <v>0</v>
       </c>
       <c r="M49" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="50" spans="1:21">
       <c r="I50" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J50" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K50" t="n">
         <v>0</v>
@@ -7222,15 +7204,15 @@
         <v>0</v>
       </c>
       <c r="M50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="51" spans="1:21">
       <c r="I51" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J51" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K51" t="n">
         <v>7</v>
@@ -7239,49 +7221,49 @@
     </row>
     <row s="55" r="52" spans="1:21">
       <c r="I52" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J52" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K52" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c s="40" r="M52" t="n"/>
     </row>
     <row s="55" r="53" spans="1:21">
       <c r="I53" t="s">
+        <v>300</v>
+      </c>
+      <c r="J53" t="s">
         <v>302</v>
       </c>
-      <c r="J53" t="s">
-        <v>304</v>
-      </c>
       <c r="K53" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c s="40" r="M53" t="n"/>
     </row>
     <row s="55" r="54" spans="1:21">
       <c r="I54" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J54" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K54" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c s="40" r="M54" t="n"/>
     </row>
     <row s="55" r="55" spans="1:21">
       <c s="36" r="I55" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c s="36" r="J55" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K55" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c s="36" r="L55" t="n"/>
       <c s="53" r="M55" t="n"/>
@@ -7293,7 +7275,7 @@
         <v>57</v>
       </c>
       <c r="J56" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K56" t="n">
         <v>0</v>
@@ -7302,7 +7284,7 @@
         <v>0</v>
       </c>
       <c r="M56" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="57" spans="1:21">
@@ -7310,7 +7292,7 @@
         <v>57</v>
       </c>
       <c r="J57" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K57" t="n">
         <v>0</v>
@@ -7319,7 +7301,7 @@
         <v>0</v>
       </c>
       <c r="M57" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="58" spans="1:21">
@@ -7327,7 +7309,7 @@
         <v>57</v>
       </c>
       <c r="J58" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K58" t="n">
         <v>0</v>
@@ -7336,7 +7318,7 @@
         <v>0</v>
       </c>
       <c r="M58" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="59" spans="1:21">
@@ -7344,7 +7326,7 @@
         <v>57</v>
       </c>
       <c r="J59" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K59" t="n">
         <v>17</v>
@@ -7355,10 +7337,10 @@
         <v>57</v>
       </c>
       <c r="J60" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K60" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row s="55" r="61" spans="1:21">
@@ -7366,10 +7348,10 @@
         <v>57</v>
       </c>
       <c r="J61" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K61" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row s="55" r="62" spans="1:21">
@@ -7377,10 +7359,10 @@
         <v>57</v>
       </c>
       <c r="J62" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K62" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row s="55" r="63" spans="1:21">
@@ -7388,18 +7370,18 @@
         <v>57</v>
       </c>
       <c r="J63" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K63" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row s="55" r="64" spans="1:21">
       <c s="13" r="I64" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c s="13" r="J64" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c s="38" r="K64" t="n">
         <v>0</v>
@@ -7408,17 +7390,17 @@
         <v>0</v>
       </c>
       <c s="38" r="M64" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c s="13" r="N64" t="n"/>
       <c s="13" r="O64" t="n"/>
     </row>
     <row s="55" r="65" spans="1:21">
       <c r="I65" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J65" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c s="39" r="K65" t="n">
         <v>-5.68e-05</v>
@@ -7427,18 +7409,18 @@
         <v>2e-07</v>
       </c>
       <c s="40" r="M65" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N65" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row hidden="1" r="66" s="55" spans="1:21">
       <c r="I66" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J66" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c s="39" r="K66" t="n">
         <v>-5.63e-05</v>
@@ -7447,18 +7429,18 @@
         <v>6e-07</v>
       </c>
       <c s="40" r="M66" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N66" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row s="55" r="67" spans="1:21">
       <c r="I67" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J67" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c s="40" r="K67" t="n">
         <v>0</v>
@@ -7470,15 +7452,15 @@
         <v>7</v>
       </c>
       <c r="N67" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row s="55" r="68" spans="1:21">
       <c r="I68" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J68" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c s="39" r="K68" t="n">
         <v>2.221e-07</v>
@@ -7490,18 +7472,18 @@
         <v>7</v>
       </c>
       <c r="N68" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O68" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="69" spans="1:21">
       <c r="I69" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J69" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c s="39" r="K69" t="n">
         <v>4.809e-07</v>
@@ -7510,21 +7492,21 @@
         <v>1.8e-07</v>
       </c>
       <c s="40" r="M69" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N69" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O69" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="70" spans="1:21">
       <c r="I70" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J70" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c s="40" r="K70" t="n">
         <v>0</v>
@@ -7536,18 +7518,18 @@
         <v>8</v>
       </c>
       <c r="N70" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O70" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="71" spans="1:21">
       <c r="I71" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J71" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c s="40" r="K71" t="n">
         <v>0</v>
@@ -7559,18 +7541,18 @@
         <v>8</v>
       </c>
       <c r="N71" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O71" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="72" spans="1:21">
       <c r="I72" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J72" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c s="40" r="K72" t="n">
         <v>0</v>
@@ -7578,46 +7560,46 @@
     </row>
     <row s="55" r="73" spans="1:21">
       <c r="I73" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J73" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c s="40" r="K73" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row s="55" r="74" spans="1:21">
       <c r="I74" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J74" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K74" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row s="55" r="75" spans="1:21">
       <c r="I75" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J75" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K75" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row s="55" r="76" spans="1:21">
       <c s="36" r="I76" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c s="36" r="J76" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K76" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c s="36" r="L76" t="n"/>
       <c s="36" r="M76" t="n"/>
@@ -7626,10 +7608,10 @@
     </row>
     <row s="55" r="77" spans="1:21">
       <c r="I77" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J77" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c s="40" r="K77" t="n">
         <v>0</v>
@@ -7638,15 +7620,15 @@
         <v>0</v>
       </c>
       <c s="40" r="M77" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="78" spans="1:21">
       <c r="I78" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J78" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c s="39" r="K78" t="n">
         <v>-5.68e-05</v>
@@ -7655,18 +7637,18 @@
         <v>2e-07</v>
       </c>
       <c s="40" r="M78" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N78" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row s="55" r="79" spans="1:21">
       <c r="I79" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J79" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c s="39" r="K79" t="n">
         <v>-5.63e-05</v>
@@ -7675,18 +7657,18 @@
         <v>6e-07</v>
       </c>
       <c s="40" r="M79" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N79" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row s="55" r="80" spans="1:21">
       <c r="I80" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J80" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c s="40" r="K80" t="n">
         <v>0</v>
@@ -7698,18 +7680,18 @@
         <v>7</v>
       </c>
       <c r="N80" t="s">
+        <v>311</v>
+      </c>
+      <c r="O80" t="s">
         <v>313</v>
-      </c>
-      <c r="O80" t="s">
-        <v>315</v>
       </c>
     </row>
     <row s="55" r="81" spans="1:21">
       <c r="I81" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J81" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c s="39" r="K81" t="n">
         <v>2.221e-07</v>
@@ -7721,18 +7703,18 @@
         <v>7</v>
       </c>
       <c r="N81" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O81" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="82" spans="1:21">
       <c r="I82" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J82" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c s="39" r="K82" t="n">
         <v>4.809e-07</v>
@@ -7741,21 +7723,21 @@
         <v>1.8e-07</v>
       </c>
       <c s="40" r="M82" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N82" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O82" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="83" spans="1:21">
       <c r="I83" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J83" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c s="40" r="K83" t="n">
         <v>0</v>
@@ -7767,18 +7749,18 @@
         <v>8</v>
       </c>
       <c r="N83" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O83" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="84" spans="1:21">
       <c r="I84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J84" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c s="40" r="K84" t="n">
         <v>0</v>
@@ -7790,15 +7772,15 @@
         <v>8</v>
       </c>
       <c r="N84" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row s="55" r="85" spans="1:21">
       <c r="I85" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J85" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c s="40" r="K85" t="n">
         <v>25</v>
@@ -7806,46 +7788,46 @@
     </row>
     <row s="55" r="86" spans="1:21">
       <c r="I86" t="s">
+        <v>321</v>
+      </c>
+      <c r="J86" t="s">
+        <v>231</v>
+      </c>
+      <c s="40" r="K86" t="s">
         <v>323</v>
-      </c>
-      <c r="J86" t="s">
-        <v>233</v>
-      </c>
-      <c s="40" r="K86" t="s">
-        <v>325</v>
       </c>
     </row>
     <row s="55" r="87" spans="1:21">
       <c r="I87" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J87" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K87" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row s="55" r="88" spans="1:21">
       <c r="I88" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J88" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K88" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row s="55" r="89" spans="1:21">
       <c s="36" r="I89" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c s="36" r="J89" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K89" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c s="14" r="L89" t="n"/>
       <c s="14" r="M89" t="n"/>
@@ -7854,10 +7836,10 @@
     </row>
     <row s="55" r="90" spans="1:21">
       <c r="I90" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J90" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c s="40" r="K90" t="n">
         <v>0</v>
@@ -7866,15 +7848,15 @@
         <v>0</v>
       </c>
       <c s="40" r="M90" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="91" spans="1:21">
       <c r="I91" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J91" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c s="39" r="K91" t="n">
         <v>-5.68e-05</v>
@@ -7883,18 +7865,18 @@
         <v>2e-07</v>
       </c>
       <c s="40" r="M91" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N91" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row s="55" r="92" spans="1:21">
       <c r="I92" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J92" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c s="39" r="K92" t="n">
         <v>-5.63e-05</v>
@@ -7903,18 +7885,18 @@
         <v>6e-07</v>
       </c>
       <c s="40" r="M92" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N92" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row s="55" r="93" spans="1:21">
       <c r="I93" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J93" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c s="40" r="K93" t="n">
         <v>0</v>
@@ -7926,18 +7908,18 @@
         <v>7</v>
       </c>
       <c r="N93" t="s">
+        <v>311</v>
+      </c>
+      <c r="O93" t="s">
         <v>313</v>
-      </c>
-      <c r="O93" t="s">
-        <v>315</v>
       </c>
     </row>
     <row s="55" r="94" spans="1:21">
       <c r="I94" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J94" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c s="39" r="K94" t="n">
         <v>2.221e-07</v>
@@ -7949,18 +7931,18 @@
         <v>7</v>
       </c>
       <c r="N94" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O94" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="95" spans="1:21">
       <c r="I95" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J95" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c s="39" r="K95" t="n">
         <v>4.809e-07</v>
@@ -7969,21 +7951,21 @@
         <v>1.8e-07</v>
       </c>
       <c s="40" r="M95" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N95" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O95" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="96" spans="1:21">
       <c r="I96" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J96" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c s="40" r="K96" t="n">
         <v>0</v>
@@ -7995,18 +7977,18 @@
         <v>8</v>
       </c>
       <c r="N96" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O96" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="97" spans="1:21">
       <c r="I97" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J97" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c s="40" r="K97" t="n">
         <v>0</v>
@@ -8018,15 +8000,15 @@
         <v>8</v>
       </c>
       <c r="N97" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row s="55" r="98" spans="1:21">
       <c r="I98" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J98" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c s="40" r="K98" t="n">
         <v>22</v>
@@ -8034,46 +8016,46 @@
     </row>
     <row s="55" r="99" spans="1:21">
       <c r="I99" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J99" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c s="40" r="K99" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row s="55" r="100" spans="1:21">
       <c r="I100" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J100" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K100" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row s="55" r="101" spans="1:21">
       <c r="I101" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J101" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K101" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row s="55" r="102" spans="1:21">
       <c s="36" r="I102" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c s="36" r="J102" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K102" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c s="36" r="L102" t="n"/>
       <c s="36" r="M102" t="n"/>
@@ -8085,7 +8067,7 @@
         <v>62</v>
       </c>
       <c r="J103" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c s="40" r="K103" t="n">
         <v>0</v>
@@ -8094,7 +8076,7 @@
         <v>0</v>
       </c>
       <c s="40" r="M103" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="104" spans="1:21">
@@ -8102,7 +8084,7 @@
         <v>62</v>
       </c>
       <c r="J104" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c s="39" r="K104" t="n">
         <v>-5.68e-05</v>
@@ -8111,10 +8093,10 @@
         <v>2e-07</v>
       </c>
       <c s="40" r="M104" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N104" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row s="55" r="105" spans="1:21">
@@ -8122,7 +8104,7 @@
         <v>62</v>
       </c>
       <c r="J105" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c s="39" r="K105" t="n">
         <v>-5.63e-05</v>
@@ -8131,10 +8113,10 @@
         <v>6e-07</v>
       </c>
       <c s="40" r="M105" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N105" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row s="55" r="106" spans="1:21">
@@ -8142,7 +8124,7 @@
         <v>62</v>
       </c>
       <c r="J106" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c s="40" r="K106" t="n">
         <v>0</v>
@@ -8154,10 +8136,10 @@
         <v>7</v>
       </c>
       <c r="N106" t="s">
+        <v>311</v>
+      </c>
+      <c r="O106" t="s">
         <v>313</v>
-      </c>
-      <c r="O106" t="s">
-        <v>315</v>
       </c>
     </row>
     <row s="55" r="107" spans="1:21">
@@ -8165,7 +8147,7 @@
         <v>62</v>
       </c>
       <c r="J107" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c s="39" r="K107" t="n">
         <v>2.221e-07</v>
@@ -8177,10 +8159,10 @@
         <v>7</v>
       </c>
       <c r="N107" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O107" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="108" spans="1:21">
@@ -8188,7 +8170,7 @@
         <v>62</v>
       </c>
       <c r="J108" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c s="39" r="K108" t="n">
         <v>4.809e-07</v>
@@ -8197,13 +8179,13 @@
         <v>1.8e-07</v>
       </c>
       <c s="40" r="M108" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N108" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O108" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="109" spans="1:21">
@@ -8211,7 +8193,7 @@
         <v>62</v>
       </c>
       <c r="J109" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c s="40" r="K109" t="n">
         <v>0</v>
@@ -8223,10 +8205,10 @@
         <v>8</v>
       </c>
       <c r="N109" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O109" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="110" spans="1:21">
@@ -8234,7 +8216,7 @@
         <v>62</v>
       </c>
       <c r="J110" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c s="40" r="K110" t="n">
         <v>0</v>
@@ -8246,7 +8228,7 @@
         <v>8</v>
       </c>
       <c r="N110" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row s="55" r="111" spans="1:21">
@@ -8254,7 +8236,7 @@
         <v>62</v>
       </c>
       <c r="J111" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K111" t="n">
         <v>23</v>
@@ -8265,10 +8247,10 @@
         <v>62</v>
       </c>
       <c r="J112" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K112" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row s="55" r="113" spans="1:21">
@@ -8276,10 +8258,10 @@
         <v>62</v>
       </c>
       <c r="J113" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K113" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row s="55" r="114" spans="1:21">
@@ -8287,10 +8269,10 @@
         <v>62</v>
       </c>
       <c r="J114" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K114" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row s="55" r="115" spans="1:21">
@@ -8298,10 +8280,10 @@
         <v>62</v>
       </c>
       <c s="36" r="J115" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K115" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c s="36" r="L115" t="n"/>
       <c s="36" r="M115" t="n"/>
@@ -8313,7 +8295,7 @@
         <v>71</v>
       </c>
       <c r="J116" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c s="40" r="K116" t="n">
         <v>0</v>
@@ -8322,7 +8304,7 @@
         <v>0</v>
       </c>
       <c s="40" r="M116" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row s="55" r="117" spans="1:21">
@@ -8330,7 +8312,7 @@
         <v>71</v>
       </c>
       <c r="J117" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c s="39" r="K117" t="n">
         <v>-5.68e-05</v>
@@ -8339,10 +8321,10 @@
         <v>2e-07</v>
       </c>
       <c s="40" r="M117" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N117" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row s="55" r="118" spans="1:21">
@@ -8350,7 +8332,7 @@
         <v>71</v>
       </c>
       <c r="J118" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c s="39" r="K118" t="n">
         <v>-5.63e-05</v>
@@ -8359,10 +8341,10 @@
         <v>6e-07</v>
       </c>
       <c s="40" r="M118" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N118" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row s="55" r="119" spans="1:21">
@@ -8370,7 +8352,7 @@
         <v>71</v>
       </c>
       <c r="J119" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c s="40" r="K119" t="n">
         <v>0</v>
@@ -8382,10 +8364,10 @@
         <v>7</v>
       </c>
       <c r="N119" t="s">
+        <v>311</v>
+      </c>
+      <c r="O119" t="s">
         <v>313</v>
-      </c>
-      <c r="O119" t="s">
-        <v>315</v>
       </c>
     </row>
     <row s="55" r="120" spans="1:21">
@@ -8393,7 +8375,7 @@
         <v>71</v>
       </c>
       <c r="J120" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c s="39" r="K120" t="n">
         <v>2.221e-07</v>
@@ -8405,10 +8387,10 @@
         <v>7</v>
       </c>
       <c r="N120" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O120" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="121" spans="1:21">
@@ -8416,7 +8398,7 @@
         <v>71</v>
       </c>
       <c r="J121" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c s="39" r="K121" t="n">
         <v>4.809e-07</v>
@@ -8425,13 +8407,13 @@
         <v>1.8e-07</v>
       </c>
       <c s="40" r="M121" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N121" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O121" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="122" spans="1:21">
@@ -8439,7 +8421,7 @@
         <v>71</v>
       </c>
       <c r="J122" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c s="40" r="K122" t="n">
         <v>0</v>
@@ -8451,10 +8433,10 @@
         <v>8</v>
       </c>
       <c r="N122" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O122" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row s="55" r="123" spans="1:21">
@@ -8462,7 +8444,7 @@
         <v>71</v>
       </c>
       <c r="J123" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c s="40" r="K123" t="n">
         <v>0</v>
@@ -8474,7 +8456,7 @@
         <v>8</v>
       </c>
       <c r="N123" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row s="55" r="124" spans="1:21">
@@ -8482,7 +8464,7 @@
         <v>71</v>
       </c>
       <c r="J124" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K124" t="n">
         <v>24</v>
@@ -8493,10 +8475,10 @@
         <v>71</v>
       </c>
       <c r="J125" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K125" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row s="55" r="126" spans="1:21">
@@ -8504,10 +8486,10 @@
         <v>71</v>
       </c>
       <c r="J126" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K126" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row s="55" r="127" spans="1:21">
@@ -8515,10 +8497,10 @@
         <v>71</v>
       </c>
       <c r="J127" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K127" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row s="55" r="128" spans="1:21">
@@ -8526,10 +8508,10 @@
         <v>71</v>
       </c>
       <c s="36" r="J128" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K128" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c s="36" r="L128" t="n"/>
       <c s="36" r="M128" t="n"/>
@@ -8541,7 +8523,7 @@
         <v>42</v>
       </c>
       <c r="J129" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K129" t="n">
         <v>2</v>
@@ -8554,10 +8536,10 @@
         <v>42</v>
       </c>
       <c r="J130" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K130" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c s="39" r="L130" t="n"/>
       <c s="40" r="M130" t="n"/>
@@ -8567,16 +8549,16 @@
         <v>42</v>
       </c>
       <c r="J131" t="s">
+        <v>338</v>
+      </c>
+      <c r="K131" t="s">
+        <v>339</v>
+      </c>
+      <c s="19" r="L131" t="s">
         <v>340</v>
       </c>
-      <c r="K131" t="s">
+      <c s="20" r="M131" t="s">
         <v>341</v>
-      </c>
-      <c s="19" r="L131" t="s">
-        <v>342</v>
-      </c>
-      <c s="20" r="M131" t="s">
-        <v>343</v>
       </c>
     </row>
     <row s="55" r="132" spans="1:21">
@@ -8584,13 +8566,13 @@
         <v>42</v>
       </c>
       <c r="J132" t="s">
+        <v>342</v>
+      </c>
+      <c r="K132" t="s">
+        <v>343</v>
+      </c>
+      <c s="19" r="L132" t="s">
         <v>344</v>
-      </c>
-      <c r="K132" t="s">
-        <v>345</v>
-      </c>
-      <c s="19" r="L132" t="s">
-        <v>346</v>
       </c>
       <c s="40" r="M132" t="n"/>
     </row>
@@ -8599,10 +8581,10 @@
         <v>42</v>
       </c>
       <c r="J133" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="K133" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c s="39" r="L133" t="n"/>
       <c s="40" r="M133" t="n"/>
@@ -8612,10 +8594,10 @@
         <v>42</v>
       </c>
       <c r="J134" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="K134" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row s="55" r="135" spans="1:21">
@@ -8623,10 +8605,10 @@
         <v>42</v>
       </c>
       <c r="J135" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K135" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row s="55" r="136" spans="1:21">
@@ -8634,10 +8616,10 @@
         <v>42</v>
       </c>
       <c s="36" r="J136" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K136" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c s="36" r="L136" t="n"/>
       <c s="36" r="M136" t="n"/>
@@ -8649,7 +8631,7 @@
         <v>32</v>
       </c>
       <c r="J137" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K137" t="n">
         <v>4</v>
@@ -8661,10 +8643,10 @@
         <v>32</v>
       </c>
       <c r="J138" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K138" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c s="39" r="L138" t="n"/>
     </row>
@@ -8673,10 +8655,10 @@
         <v>32</v>
       </c>
       <c r="J139" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K139" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c s="39" r="L139" t="n"/>
     </row>
@@ -8685,13 +8667,13 @@
         <v>32</v>
       </c>
       <c r="J140" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="K140" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c s="19" r="L140" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row s="55" r="141" spans="1:21">
@@ -8699,10 +8681,10 @@
         <v>32</v>
       </c>
       <c r="J141" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="K141" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c s="39" r="L141" t="n"/>
     </row>
@@ -8711,10 +8693,10 @@
         <v>32</v>
       </c>
       <c r="J142" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="K142" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row s="55" r="143" spans="1:21">
@@ -8722,13 +8704,13 @@
         <v>32</v>
       </c>
       <c r="J143" t="s">
+        <v>357</v>
+      </c>
+      <c r="K143" t="s">
+        <v>358</v>
+      </c>
+      <c r="L143" t="s">
         <v>359</v>
-      </c>
-      <c r="K143" t="s">
-        <v>360</v>
-      </c>
-      <c r="L143" t="s">
-        <v>361</v>
       </c>
     </row>
     <row s="55" r="144" spans="1:21">
@@ -8736,10 +8718,10 @@
         <v>32</v>
       </c>
       <c r="J144" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K144" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row s="55" r="145" spans="1:21">
@@ -8747,10 +8729,10 @@
         <v>32</v>
       </c>
       <c s="36" r="J145" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c s="36" r="K145" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c s="36" r="L145" t="n"/>
       <c s="36" r="M145" t="n"/>
@@ -8806,7 +8788,7 @@
   <sheetData>
     <row s="55" r="1" spans="1:25">
       <c s="15" r="A1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c s="15" r="B1" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
Parameters or data update
</commit_message>
<xml_diff>
--- a/HRBC_template.xlsx
+++ b/HRBC_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="12150" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="12150" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Comments" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Parameters" sheetId="4" r:id="rId4"/>
     <sheet name="Results" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -3251,7 +3251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="765" topLeftCell="A37" activePane="bottomLeft"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="AE80" sqref="AE80"/>
@@ -12038,10 +12038,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U171"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="540" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="540" topLeftCell="A28" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="O90" sqref="O90"/>
+      <selection pane="bottomLeft" activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minor tweak of no consequence
</commit_message>
<xml_diff>
--- a/HRBC_template.xlsx
+++ b/HRBC_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\MSL\Private\Electricity\Staff\TBL\GitHub\HRBC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A597ED3A-E21A-4320-8541-3054D08B4B81}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E3EF3698-3F89-441B-874A-404D88B3252B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="12150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="12150" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comments" sheetId="1" r:id="rId1"/>
@@ -1350,9 +1350,6 @@
     <t>UNUSED HP3458A, s/n382</t>
   </si>
   <si>
-    <t>HRBC.v1.0 G493 100k:SR104r 10k 03/03/2017 11:37:33</t>
-  </si>
-  <si>
     <t>Relay del.</t>
   </si>
   <si>
@@ -1384,6 +1381,9 @@
   </si>
   <si>
     <t>T (°C)</t>
+  </si>
+  <si>
+    <t>HRBC.v2.0 G493 100k:SR104r 10k 03/03/2017 11:37:33</t>
   </si>
 </sst>
 </file>
@@ -2520,10 +2520,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI120"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="765" activePane="bottomLeft"/>
       <selection activeCell="AA1" sqref="AA1:AB1048576"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2581,7 +2581,7 @@
         <v>63</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>433</v>
+        <v>444</v>
       </c>
       <c r="G4" s="73"/>
       <c r="H4" s="84" t="s">
@@ -2593,19 +2593,19 @@
       </c>
       <c r="K4" s="84"/>
       <c r="L4" s="84" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M4" s="84"/>
       <c r="N4" s="84" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="O4" s="84"/>
       <c r="P4" s="84" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q4" s="84"/>
       <c r="R4" s="84" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="S4" s="84"/>
       <c r="T4" t="s">
@@ -2626,7 +2626,7 @@
       <c r="Y4" s="84"/>
       <c r="Z4" s="84"/>
       <c r="AA4" s="71" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AB4" s="71" t="s">
         <v>60</v>
@@ -2658,58 +2658,58 @@
         <v>51</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I5" t="s">
         <v>65</v>
       </c>
       <c r="J5" s="71" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K5" s="71" t="s">
         <v>65</v>
       </c>
       <c r="L5" s="71" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="M5" s="71" t="s">
         <v>65</v>
       </c>
       <c r="N5" s="71" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="O5" t="s">
         <v>65</v>
       </c>
       <c r="P5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Q5" t="s">
         <v>65</v>
       </c>
       <c r="R5" s="71" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="S5" s="71" t="s">
         <v>65</v>
       </c>
       <c r="T5" s="28" t="s">
+        <v>441</v>
+      </c>
+      <c r="U5" s="71" t="s">
+        <v>441</v>
+      </c>
+      <c r="V5" s="71" t="s">
         <v>442</v>
       </c>
-      <c r="U5" s="71" t="s">
+      <c r="W5" s="71" t="s">
         <v>442</v>
       </c>
-      <c r="V5" s="71" t="s">
+      <c r="X5" s="72" t="s">
         <v>443</v>
-      </c>
-      <c r="W5" s="71" t="s">
-        <v>443</v>
-      </c>
-      <c r="X5" s="72" t="s">
-        <v>444</v>
       </c>
       <c r="Y5" s="72" t="s">
         <v>67</v>
@@ -3022,7 +3022,7 @@
       <c r="V12"/>
       <c r="Z12"/>
       <c r="AC12" s="12" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AD12" s="13" t="s">
         <v>81</v>
@@ -6431,8 +6431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U189"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="540" activePane="bottomLeft"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="540" topLeftCell="A92" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft" activeCell="K135" sqref="K135"/>
     </sheetView>

</xml_diff>

<commit_message>
Corrected default GMH DLL path
Corrected path to new location (...\Electricity - Ongoing\...)
</commit_message>
<xml_diff>
--- a/HRBC_template.xlsx
+++ b/HRBC_template.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="722">
   <si>
     <t>WARNING: DO NOT INSERT ANY COMMENTS IN THIS WORKBOOK!</t>
   </si>
@@ -866,31 +866,31 @@
     <t>R1: CHANGE_THIS! 1G monitored by GMH: s/n627. R2: CHANGE_THIS! 1M monitored by GMH: s/n628</t>
   </si>
   <si>
-    <t>03/08/2017 11:58:30</t>
-  </si>
-  <si>
-    <t>03/08/2017 12:0:3</t>
-  </si>
-  <si>
-    <t>03/08/2017 11:57:17</t>
-  </si>
-  <si>
-    <t>03/08/2017 12:4:4</t>
-  </si>
-  <si>
-    <t>03/08/2017 12:5:37</t>
-  </si>
-  <si>
-    <t>03/08/2017 12:2:51</t>
-  </si>
-  <si>
-    <t>03/08/2017 12:9:37</t>
-  </si>
-  <si>
-    <t>03/08/2017 12:11:10</t>
-  </si>
-  <si>
-    <t>03/08/2017 12:8:24</t>
+    <t>06/12/2019 11:56:29</t>
+  </si>
+  <si>
+    <t>06/12/2019 11:57:52</t>
+  </si>
+  <si>
+    <t>06/12/2019 11:55:25</t>
+  </si>
+  <si>
+    <t>06/12/2019 12:01:44</t>
+  </si>
+  <si>
+    <t>06/12/2019 12:03:07</t>
+  </si>
+  <si>
+    <t>06/12/2019 12:00:40</t>
+  </si>
+  <si>
+    <t>06/12/2019 12:06:57</t>
+  </si>
+  <si>
+    <t>06/12/2019 12:08:20</t>
+  </si>
+  <si>
+    <t>06/12/2019 12:05:53</t>
   </si>
   <si>
     <t>03/08/2017 12:15:10</t>
@@ -2184,33 +2184,6 @@
   </si>
   <si>
     <t>02/08/2017 18:45:35</t>
-  </si>
-  <si>
-    <t>06/12/2019 11:56:29</t>
-  </si>
-  <si>
-    <t>06/12/2019 11:57:52</t>
-  </si>
-  <si>
-    <t>06/12/2019 11:55:25</t>
-  </si>
-  <si>
-    <t>06/12/2019 12:01:44</t>
-  </si>
-  <si>
-    <t>06/12/2019 12:03:07</t>
-  </si>
-  <si>
-    <t>06/12/2019 12:00:40</t>
-  </si>
-  <si>
-    <t>06/12/2019 12:06:57</t>
-  </si>
-  <si>
-    <t>06/12/2019 12:08:20</t>
-  </si>
-  <si>
-    <t>06/12/2019 12:05:53</t>
   </si>
 </sst>
 </file>
@@ -8004,7 +7977,7 @@
         <v>60</v>
       </c>
       <c r="G72" t="s">
-        <v>722</v>
+        <v>282</v>
       </c>
       <c s="9" r="H72" t="n">
         <v>1.000011625836011</v>
@@ -8022,7 +7995,7 @@
         <v>0</v>
       </c>
       <c r="M72" t="s">
-        <v>723</v>
+        <v>283</v>
       </c>
       <c s="39" r="N72" t="n">
         <v>5.789047207620459e-07</v>
@@ -8031,7 +8004,7 @@
         <v>1.303981154808418e-06</v>
       </c>
       <c r="P72" t="s">
-        <v>724</v>
+        <v>284</v>
       </c>
       <c s="9" r="Q72" t="n">
         <v>-9.999974576601758</v>
@@ -8090,7 +8063,7 @@
         <v>60</v>
       </c>
       <c r="G73" t="s">
-        <v>725</v>
+        <v>285</v>
       </c>
       <c s="9" r="H73" t="n">
         <v>-1.000017790904014</v>
@@ -8108,7 +8081,7 @@
         <v>0</v>
       </c>
       <c r="M73" t="s">
-        <v>726</v>
+        <v>286</v>
       </c>
       <c s="39" r="N73" t="n">
         <v>-1.125329498184024e-07</v>
@@ -8117,7 +8090,7 @@
         <v>7.1758534136079e-07</v>
       </c>
       <c r="P73" t="s">
-        <v>727</v>
+        <v>287</v>
       </c>
       <c s="9" r="Q73" t="n">
         <v>10.0000246461447</v>
@@ -8176,7 +8149,7 @@
         <v>60</v>
       </c>
       <c r="G74" t="s">
-        <v>728</v>
+        <v>288</v>
       </c>
       <c s="9" r="H74" t="n">
         <v>-1.001005023182846</v>
@@ -8194,7 +8167,7 @@
         <v>0</v>
       </c>
       <c r="M74" t="s">
-        <v>729</v>
+        <v>289</v>
       </c>
       <c s="39" r="N74" t="n">
         <v>-1.568699366007855e-07</v>
@@ -8203,7 +8176,7 @@
         <v>9.438703928905606e-07</v>
       </c>
       <c r="P74" t="s">
-        <v>730</v>
+        <v>290</v>
       </c>
       <c s="9" r="Q74" t="n">
         <v>9.999988425603686</v>

</xml_diff>